<commit_message>
Allow for swapped polarity on 4G63 decoder
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/v0.4_bom.xlsx
+++ b/reference/hardware/v0.4/v0.4_bom.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="223">
   <si>
     <t>Value</t>
   </si>
@@ -516,9 +516,6 @@
     <t>C11,12,20</t>
   </si>
   <si>
-    <t>Digikey import</t>
-  </si>
-  <si>
     <t>Dual Terminal Block</t>
   </si>
   <si>
@@ -748,6 +745,12 @@
   </si>
   <si>
     <t>J4</t>
+  </si>
+  <si>
+    <t>Full Digikey import</t>
+  </si>
+  <si>
+    <t>2Ch Digikey import</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1451,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="N31" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1464,22 +1467,22 @@
     <col min="12" max="12" width="17.1640625" customWidth="1"/>
     <col min="13" max="13" width="28" customWidth="1"/>
     <col min="17" max="17" width="47.83203125" customWidth="1"/>
-    <col min="18" max="18" width="27.33203125" customWidth="1"/>
-    <col min="19" max="19" width="28" customWidth="1"/>
+    <col min="18" max="19" width="27.33203125" customWidth="1"/>
+    <col min="20" max="20" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1491,7 +1494,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1500,7 +1503,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1512,22 +1515,25 @@
         <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="4"/>
@@ -1549,12 +1555,16 @@
         <f>IF(NOT(M2=""),A2&amp;","&amp;M2,"")</f>
         <v/>
       </c>
-      <c r="S2" t="str">
+      <c r="S2" s="4" t="str">
+        <f>IF(NOT(N2=""),B2&amp;","&amp;N2,"")</f>
+        <v/>
+      </c>
+      <c r="T2" t="str">
         <f>A2&amp;"x "&amp;E2</f>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <f>LEN(C3)-LEN(SUBSTITUTE(C3,",",""))+1</f>
         <v>1</v>
@@ -1573,7 +1583,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>10</v>
@@ -1586,13 +1596,13 @@
         <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="N3" s="5">
         <v>1.7</v>
@@ -1607,15 +1617,19 @@
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="str">
-        <f t="shared" ref="R3:R51" si="2">IF(NOT(M3=""),A3&amp;","&amp;M3,"")</f>
+        <f t="shared" ref="R3:S51" si="2">IF(NOT(M3=""),A3&amp;","&amp;M3,"")</f>
         <v>1,399-3654-ND</v>
       </c>
-      <c r="S3" t="str">
+      <c r="S3" s="4" t="str">
+        <f>IF(NOT(M3=""),B3&amp;","&amp;M3,"")</f>
+        <v>1,399-3654-ND</v>
+      </c>
+      <c r="T3" t="str">
         <f>"Capacitor - " &amp;A3&amp;"x "&amp;E3</f>
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>LEN(C4)-LEN(SUBSTITUTE(C4,",",""))+1</f>
         <v>5</v>
@@ -1634,7 +1648,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>13</v>
@@ -1647,13 +1661,13 @@
         <v>14</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N4" s="5">
         <v>0.66</v>
@@ -1671,12 +1685,16 @@
         <f t="shared" si="2"/>
         <v>5,399-4353-ND</v>
       </c>
-      <c r="S4" t="str">
-        <f t="shared" ref="S4:S10" si="4">"Capacitor - " &amp;A4&amp;"x "&amp;E4</f>
+      <c r="S4" s="4" t="str">
+        <f t="shared" ref="S4:S48" si="4">IF(NOT(M4=""),B4&amp;","&amp;M4,"")</f>
+        <v>5,399-4353-ND</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" ref="T4:T10" si="5">"Capacitor - " &amp;A4&amp;"x "&amp;E4</f>
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f>LEN(C5)-LEN(SUBSTITUTE(C5,",",""))+1</f>
         <v>7</v>
@@ -1695,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>13</v>
@@ -1708,13 +1726,13 @@
         <v>14</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="N5" s="5">
         <v>0.32</v>
@@ -1732,12 +1750,16 @@
         <f t="shared" si="2"/>
         <v>7,399-9879-1-ND</v>
       </c>
-      <c r="S5" t="str">
+      <c r="S5" s="4" t="str">
         <f t="shared" si="4"/>
+        <v>7,399-9879-1-ND</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="5"/>
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f>LEN(C6)-LEN(SUBSTITUTE(C6,",",""))+1</f>
         <v>1</v>
@@ -1756,7 +1778,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>10</v>
@@ -1769,13 +1791,13 @@
         <v>14</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="N6" s="5">
         <v>1.57</v>
@@ -1793,14 +1815,18 @@
         <f t="shared" si="2"/>
         <v>1,399-3652-ND</v>
       </c>
-      <c r="S6" t="str">
+      <c r="S6" s="4" t="str">
         <f t="shared" si="4"/>
+        <v>1,399-3652-ND</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="5"/>
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
-        <f t="shared" ref="A7:A9" si="5">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
+        <f t="shared" ref="A7:A9" si="6">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B7" s="20">
@@ -1817,7 +1843,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
@@ -1830,13 +1856,13 @@
         <v>11</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="N7" s="5">
         <v>0.62</v>
@@ -1854,14 +1880,18 @@
         <f t="shared" si="2"/>
         <v>1,478-5120-ND</v>
       </c>
-      <c r="S7" t="str">
+      <c r="S7" s="4" t="str">
         <f t="shared" si="4"/>
+        <v>1,478-5120-ND</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="5"/>
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B8" s="20">
@@ -1878,7 +1908,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
@@ -1891,13 +1921,13 @@
         <v>14</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="N8" s="5">
         <v>0.24</v>
@@ -1915,14 +1945,18 @@
         <f t="shared" si="2"/>
         <v>1,399-4206-ND</v>
       </c>
-      <c r="S8" t="str">
+      <c r="S8" s="4" t="str">
         <f t="shared" si="4"/>
+        <v>1,399-4206-ND</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="5"/>
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="B9" s="20">
@@ -1933,13 +1967,13 @@
         <v>143</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>13</v>
@@ -1952,13 +1986,13 @@
         <v>14</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="N9" s="5">
         <v>0.66</v>
@@ -1976,12 +2010,16 @@
         <f t="shared" si="2"/>
         <v>3,399-4390-ND</v>
       </c>
-      <c r="S9" t="str">
+      <c r="S9" s="4" t="str">
         <f t="shared" si="4"/>
+        <v>2,399-4390-ND</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="5"/>
         <v>Capacitor - 3x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f>LEN(C10)-LEN(SUBSTITUTE(C10,",",""))+1</f>
         <v>1</v>
@@ -2011,7 +2049,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>141</v>
@@ -2035,12 +2073,16 @@
         <f t="shared" si="2"/>
         <v>1,399-4243-ND</v>
       </c>
-      <c r="S10" t="str">
+      <c r="S10" s="4" t="str">
         <f t="shared" si="4"/>
+        <v>1,399-4243-ND</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="5"/>
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="4"/>
@@ -2065,8 +2107,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S11" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="4"/>
@@ -2091,14 +2137,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <f>LEN(C13)-LEN(SUBSTITUTE(C13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B13" s="20">
-        <f t="shared" ref="B13:B16" si="6">LEN(D13)-LEN(SUBSTITUTE(D13,",",""))+1</f>
+        <f t="shared" ref="B13:B16" si="7">LEN(D13)-LEN(SUBSTITUTE(D13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2108,7 +2158,7 @@
         <v>93</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>20</v>
@@ -2124,7 +2174,7 @@
         <v>22</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>23</v>
@@ -2148,18 +2198,22 @@
         <f t="shared" si="2"/>
         <v>1,1N5919BGOS-ND</v>
       </c>
-      <c r="S13" t="str">
+      <c r="S13" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,1N5919BGOS-ND</v>
+      </c>
+      <c r="T13" t="str">
         <f>"Diode - " &amp;A13&amp;"x "&amp;E13</f>
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <f>LEN(C14)-LEN(SUBSTITUTE(C14,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B14" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -2169,7 +2223,7 @@
         <v>131</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>26</v>
@@ -2185,7 +2239,7 @@
         <v>27</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>25</v>
@@ -2209,25 +2263,29 @@
         <f t="shared" si="2"/>
         <v>12,1N5818-TPCT-ND</v>
       </c>
-      <c r="S14" t="str">
-        <f t="shared" ref="S14:S16" si="7">"Diode - " &amp;A14&amp;"x "&amp;E14</f>
+      <c r="S14" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>12,1N5818-TPCT-ND</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" ref="T14:T16" si="8">"Diode - " &amp;A14&amp;"x "&amp;E14</f>
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <f>LEN(C15)-LEN(SUBSTITUTE(C15,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B15" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>92</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>29</v>
@@ -2242,7 +2300,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="2" t="s">
@@ -2264,25 +2322,29 @@
         <f t="shared" si="2"/>
         <v>8,160-1139-ND</v>
       </c>
-      <c r="S15" t="str">
-        <f t="shared" si="7"/>
+      <c r="S15" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>4,160-1139-ND</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="8"/>
         <v>Diode - 8x LED-Red</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <f>LEN(C16)-LEN(SUBSTITUTE(C16,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B16" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>30</v>
@@ -2301,7 +2363,7 @@
         <v>27</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>32</v>
@@ -2325,12 +2387,16 @@
         <f t="shared" si="2"/>
         <v>4,1N4004-TPMSCT-ND</v>
       </c>
-      <c r="S16" t="str">
-        <f t="shared" si="7"/>
+      <c r="S16" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>2,1N4004-TPMSCT-ND</v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" si="8"/>
         <v>Diode - 4x 1N4004</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="4"/>
@@ -2355,12 +2421,16 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="S17" t="str">
-        <f t="shared" ref="S17:S46" si="8">A17&amp;"x "&amp;E17</f>
+      <c r="S17" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" ref="T17:T46" si="9">A17&amp;"x "&amp;E17</f>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="4"/>
@@ -2385,12 +2455,16 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="S18" t="str">
-        <f t="shared" si="8"/>
+      <c r="S18" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="9"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="4"/>
@@ -2415,17 +2489,21 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="S19" t="str">
-        <f t="shared" si="8"/>
+      <c r="S19" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="9"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>1</v>
       </c>
       <c r="B20" s="20">
-        <f t="shared" ref="B20" si="9">LEN(D20)-LEN(SUBSTITUTE(D20,",",""))+1</f>
+        <f t="shared" ref="B20" si="10">LEN(D20)-LEN(SUBSTITUTE(D20,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2451,7 +2529,7 @@
         <v>37</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>38</v>
@@ -2475,12 +2553,16 @@
         <f t="shared" si="2"/>
         <v>1,P7307-ND</v>
       </c>
-      <c r="S20" t="str">
-        <f t="shared" si="8"/>
+      <c r="S20" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,P7307-ND</v>
+      </c>
+      <c r="T20" t="str">
+        <f t="shared" si="9"/>
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="4"/>
@@ -2505,17 +2587,21 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="S21" t="str">
-        <f t="shared" si="8"/>
+      <c r="S21" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T21" t="str">
+        <f t="shared" si="9"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>1</v>
       </c>
       <c r="B22" s="20">
-        <f t="shared" ref="B22" si="10">LEN(D22)-LEN(SUBSTITUTE(D22,",",""))+1</f>
+        <f t="shared" ref="B22" si="11">LEN(D22)-LEN(SUBSTITUTE(D22,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -2525,7 +2611,7 @@
         <v>135</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>134</v>
@@ -2537,7 +2623,7 @@
         <v>133</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>136</v>
@@ -2563,12 +2649,16 @@
         <f t="shared" si="2"/>
         <v>1,ED2561-ND</v>
       </c>
-      <c r="S22" t="str">
+      <c r="S22" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,ED2561-ND</v>
+      </c>
+      <c r="T22" t="str">
         <f>A22&amp;"x "&amp;E22</f>
         <v>1x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>5</v>
       </c>
@@ -2592,7 +2682,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="2" t="s">
@@ -2614,12 +2704,16 @@
         <f t="shared" si="2"/>
         <v>5,3M9580-ND</v>
       </c>
-      <c r="S23" t="str">
-        <f t="shared" si="8"/>
+      <c r="S23" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>5,3M9580-ND</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="9"/>
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>2</v>
       </c>
@@ -2633,7 +2727,7 @@
         <v>115</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>129</v>
@@ -2647,7 +2741,7 @@
         <v>128</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>127</v>
@@ -2671,12 +2765,16 @@
         <f t="shared" si="2"/>
         <v>2,S1012EC-40-ND</v>
       </c>
-      <c r="S24" t="str">
-        <f t="shared" si="8"/>
+      <c r="S24" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>2,S1012EC-40-ND</v>
+      </c>
+      <c r="T24" t="str">
+        <f t="shared" si="9"/>
         <v>2x 40 POS 0.100 Pin Header</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="53" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>1</v>
       </c>
@@ -2684,16 +2782,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -2701,16 +2799,16 @@
         <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="M25" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N25" s="6">
         <v>1.1299999999999999</v>
@@ -2720,20 +2818,24 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="P25" s="6">
-        <f t="shared" ref="P25" si="11">N25*B25</f>
+        <f t="shared" ref="P25" si="12">N25*B25</f>
         <v>1.1299999999999999</v>
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="4" t="str">
-        <f t="shared" ref="R25" si="12">IF(NOT(M25=""),A25&amp;","&amp;M25,"")</f>
+        <f t="shared" ref="R25:S25" si="13">IF(NOT(M25=""),A25&amp;","&amp;M25,"")</f>
         <v>1,1175-1614-ND</v>
       </c>
-      <c r="S25" t="str">
-        <f t="shared" ref="S25" si="13">A25&amp;"x "&amp;E25</f>
+      <c r="S25" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,1175-1614-ND</v>
+      </c>
+      <c r="T25" t="str">
+        <f t="shared" ref="T25" si="14">A25&amp;"x "&amp;E25</f>
         <v>1x Rectangular Connectors - Headers, Male Pins</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="4"/>
@@ -2755,12 +2857,16 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="S26" t="str">
-        <f t="shared" si="8"/>
+      <c r="S26" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="9"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="4"/>
@@ -2782,28 +2888,32 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="S27" t="str">
-        <f t="shared" si="8"/>
+      <c r="S27" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T27" t="str">
+        <f t="shared" si="9"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <f>LEN(C28)-LEN(SUBSTITUTE(C28,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B28" s="20">
-        <f t="shared" ref="B28" si="14">LEN(D28)-LEN(SUBSTITUTE(D28,",",""))+1</f>
+        <f t="shared" ref="B28" si="15">LEN(D28)-LEN(SUBSTITUTE(D28,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>108</v>
@@ -2819,7 +2929,7 @@
         <v>41</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>109</v>
@@ -2843,12 +2953,16 @@
         <f t="shared" si="2"/>
         <v>8,497-5896-5-ND</v>
       </c>
-      <c r="S28" t="str">
-        <f t="shared" si="8"/>
+      <c r="S28" s="4" t="str">
+        <f>IF(NOT(M28=""),B28&amp;","&amp;M28,"")</f>
+        <v>6,497-5896-5-ND</v>
+      </c>
+      <c r="T28" t="str">
+        <f t="shared" si="9"/>
         <v>8x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="4"/>
@@ -2870,8 +2984,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S29" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="4"/>
@@ -2893,14 +3011,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S30" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <f>LEN(C31)-LEN(SUBSTITUTE(C31,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B31" s="20">
-        <f t="shared" ref="B31:B37" si="15">LEN(D31)-LEN(SUBSTITUTE(D31,",",""))+1</f>
+        <f t="shared" ref="B31:B37" si="16">LEN(D31)-LEN(SUBSTITUTE(D31,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -2924,7 +3046,7 @@
         <v>44</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>45</v>
@@ -2936,7 +3058,7 @@
         <v>0.08</v>
       </c>
       <c r="O31" s="6">
-        <f t="shared" ref="O31:O39" si="16">N31*A31</f>
+        <f t="shared" ref="O31:O39" si="17">N31*A31</f>
         <v>0.4</v>
       </c>
       <c r="P31" s="6">
@@ -2948,25 +3070,29 @@
         <f t="shared" si="2"/>
         <v>5,10.0KXBK-ND</v>
       </c>
-      <c r="S31" t="str">
+      <c r="S31" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>5,10.0KXBK-ND</v>
+      </c>
+      <c r="T31" t="str">
         <f>"Resistor - " &amp; A31&amp;"x "&amp;E31</f>
         <v>Resistor - 5x 10k</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <f>LEN(C32)-LEN(SUBSTITUTE(C32,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B32" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>121</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>47</v>
@@ -2983,7 +3109,7 @@
         <v>44</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>49</v>
@@ -2995,7 +3121,7 @@
         <v>0.06</v>
       </c>
       <c r="O32" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.72</v>
       </c>
       <c r="P32" s="6">
@@ -3007,50 +3133,54 @@
         <f t="shared" si="2"/>
         <v>12,1.00KXBK-ND</v>
       </c>
-      <c r="S32" t="str">
-        <f t="shared" ref="S32:S39" si="17">"Resistor - " &amp; A32&amp;"x "&amp;E32</f>
+      <c r="S32" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>8,1.00KXBK-ND</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" ref="T32:T39" si="18">"Resistor - " &amp; A32&amp;"x "&amp;E32</f>
         <v>Resistor - 12x 1k</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <f>LEN(C33)-LEN(SUBSTITUTE(C33,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B33" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>116</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E33" s="13">
         <v>680</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L33" s="7"/>
       <c r="M33" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N33" s="14">
         <v>0.22</v>
       </c>
       <c r="O33" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.76</v>
       </c>
       <c r="P33" s="6">
@@ -3064,25 +3194,29 @@
         <f t="shared" si="2"/>
         <v>8,A105963CT-ND</v>
       </c>
-      <c r="S33" t="str">
-        <f t="shared" si="17"/>
+      <c r="S33" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>4,A105963CT-ND</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="18"/>
         <v>Resistor - 8x 680</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <f>LEN(C34)-LEN(SUBSTITUTE(C34,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="B34" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E34" s="3">
         <v>470</v>
@@ -3099,7 +3233,7 @@
         <v>52</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>53</v>
@@ -3111,7 +3245,7 @@
         <v>0.11</v>
       </c>
       <c r="O34" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.66</v>
       </c>
       <c r="P34" s="6">
@@ -3123,17 +3257,21 @@
         <f t="shared" si="2"/>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
-      <c r="S34" t="str">
-        <f t="shared" si="17"/>
+      <c r="S34" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>6,RNF14FTD470RCT-ND</v>
+      </c>
+      <c r="T34" t="str">
+        <f t="shared" si="18"/>
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>2</v>
       </c>
       <c r="B35" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -3143,7 +3281,7 @@
         <v>86</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>55</v>
@@ -3159,7 +3297,7 @@
         <v>57</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>58</v>
@@ -3171,7 +3309,7 @@
         <v>1.92</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3.84</v>
       </c>
       <c r="P35" s="6">
@@ -3183,17 +3321,21 @@
         <f t="shared" si="2"/>
         <v>2,985-1047-1-ND</v>
       </c>
-      <c r="S35" t="str">
-        <f t="shared" si="17"/>
+      <c r="S35" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>2,985-1047-1-ND</v>
+      </c>
+      <c r="T35" t="str">
+        <f t="shared" si="18"/>
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>1</v>
       </c>
       <c r="B36" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -3203,7 +3345,7 @@
         <v>87</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>60</v>
@@ -3217,7 +3359,7 @@
         <v>44</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>61</v>
@@ -3229,7 +3371,7 @@
         <v>0.46</v>
       </c>
       <c r="O36" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.46</v>
       </c>
       <c r="P36" s="6">
@@ -3243,17 +3385,21 @@
         <f t="shared" si="2"/>
         <v>1,3.9KADCT-ND</v>
       </c>
-      <c r="S36" t="str">
-        <f t="shared" si="17"/>
+      <c r="S36" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,3.9KADCT-ND</v>
+      </c>
+      <c r="T36" t="str">
+        <f t="shared" si="18"/>
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>1</v>
       </c>
       <c r="B37" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -3263,7 +3409,7 @@
         <v>88</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>63</v>
@@ -3277,7 +3423,7 @@
         <v>44</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>64</v>
@@ -3289,7 +3435,7 @@
         <v>0.46</v>
       </c>
       <c r="O37" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.46</v>
       </c>
       <c r="P37" s="6">
@@ -3303,14 +3449,18 @@
         <f t="shared" si="2"/>
         <v>1,1KADCT-ND</v>
       </c>
-      <c r="S37" t="str">
-        <f t="shared" si="17"/>
+      <c r="S37" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,1KADCT-ND</v>
+      </c>
+      <c r="T37" t="str">
+        <f t="shared" si="18"/>
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
-        <f t="shared" ref="A38:A39" si="18">LEN(C38)-LEN(SUBSTITUTE(C38,",",""))+1</f>
+        <f t="shared" ref="A38:A39" si="19">LEN(C38)-LEN(SUBSTITUTE(C38,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B38" s="20">
@@ -3321,7 +3471,7 @@
         <v>123</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>66</v>
@@ -3338,7 +3488,7 @@
         <v>44</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>68</v>
@@ -3350,7 +3500,7 @@
         <v>0.1</v>
       </c>
       <c r="O38" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="P38" s="6">
@@ -3362,14 +3512,18 @@
         <f t="shared" si="2"/>
         <v>12,100KXBK-ND</v>
       </c>
-      <c r="S38" t="str">
-        <f t="shared" si="17"/>
+      <c r="S38" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>8,100KXBK-ND</v>
+      </c>
+      <c r="T38" t="str">
+        <f t="shared" si="18"/>
         <v>Resistor - 12x 100k</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="B39" s="20">
@@ -3380,7 +3534,7 @@
         <v>89</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E39" s="3">
         <v>160</v>
@@ -3397,7 +3551,7 @@
         <v>44</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>71</v>
@@ -3409,7 +3563,7 @@
         <v>0.27</v>
       </c>
       <c r="O39" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.08</v>
       </c>
       <c r="P39" s="6">
@@ -3421,12 +3575,16 @@
         <f t="shared" si="2"/>
         <v>4,160YCT-ND</v>
       </c>
-      <c r="S39" t="str">
-        <f t="shared" si="17"/>
+      <c r="S39" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>2,160YCT-ND</v>
+      </c>
+      <c r="T39" t="str">
+        <f t="shared" si="18"/>
         <v>Resistor - 4x 160</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="4"/>
@@ -3448,8 +3606,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S40" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="4"/>
@@ -3471,13 +3633,17 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S41" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>1</v>
       </c>
       <c r="B42" s="20">
-        <f t="shared" ref="B42:B44" si="19">LEN(D42)-LEN(SUBSTITUTE(D42,",",""))+1</f>
+        <f t="shared" ref="B42:B44" si="20">LEN(D42)-LEN(SUBSTITUTE(D42,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -3503,7 +3669,7 @@
         <v>78</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>75</v>
@@ -3527,17 +3693,21 @@
         <f t="shared" si="2"/>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
-      <c r="S42" t="str">
-        <f t="shared" si="8"/>
+      <c r="S42" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,LM2940T-5.0/NOPB</v>
+      </c>
+      <c r="T42" t="str">
+        <f t="shared" si="9"/>
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>1</v>
       </c>
       <c r="B43" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -3547,7 +3717,7 @@
         <v>99</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>98</v>
@@ -3583,33 +3753,37 @@
         <f t="shared" si="2"/>
         <v>1,MPX4250AP-ND</v>
       </c>
-      <c r="S43" t="str">
-        <f t="shared" si="8"/>
+      <c r="S43" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,MPX4250AP-ND</v>
+      </c>
+      <c r="T43" t="str">
+        <f t="shared" si="9"/>
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>2</v>
       </c>
       <c r="B44" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="C44" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E44" s="13" t="s">
+      <c r="F44" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="G44" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="13">
@@ -3619,11 +3793,11 @@
         <v>79</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L44" s="13"/>
       <c r="M44" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N44" s="23">
         <v>2.92</v>
@@ -3641,12 +3815,16 @@
         <f t="shared" si="2"/>
         <v>2,TC4424EPA-ND</v>
       </c>
-      <c r="S44" t="str">
-        <f t="shared" si="8"/>
+      <c r="S44" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,TC4424EPA-ND</v>
+      </c>
+      <c r="T44" t="str">
+        <f t="shared" si="9"/>
         <v>2x TC4424EPA</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22">
         <v>1</v>
       </c>
@@ -3654,33 +3832,33 @@
         <v>1</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13">
         <v>1</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L45" s="13"/>
       <c r="M45" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N45" s="23">
         <v>0.72</v>
@@ -3690,20 +3868,24 @@
         <v>0.72</v>
       </c>
       <c r="P45" s="6">
-        <f t="shared" ref="P45" si="20">N45*B45</f>
+        <f t="shared" ref="P45" si="21">N45*B45</f>
         <v>0.72</v>
       </c>
       <c r="Q45" s="12"/>
       <c r="R45" s="4" t="str">
-        <f t="shared" ref="R45" si="21">IF(NOT(M45=""),A45&amp;","&amp;M45,"")</f>
+        <f t="shared" ref="R45:S45" si="22">IF(NOT(M45=""),A45&amp;","&amp;M45,"")</f>
         <v>1,ULN2803APGCN-ND</v>
       </c>
-      <c r="S45" t="str">
-        <f t="shared" ref="S45" si="22">A45&amp;"x "&amp;E45</f>
+      <c r="S45" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,ULN2803APGCN-ND</v>
+      </c>
+      <c r="T45" t="str">
+        <f t="shared" ref="T45" si="23">A45&amp;"x "&amp;E45</f>
         <v>1x ULN2803APG</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <v>3</v>
       </c>
@@ -3717,7 +3899,7 @@
         <v>102</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -3725,7 +3907,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>101</v>
@@ -3749,12 +3931,16 @@
         <f t="shared" si="2"/>
         <v>3,AE10011-ND</v>
       </c>
-      <c r="S46" t="str">
-        <f t="shared" si="8"/>
+      <c r="S46" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>2,AE10011-ND</v>
+      </c>
+      <c r="T46" t="str">
+        <f t="shared" si="9"/>
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="4"/>
@@ -3776,8 +3962,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S47" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>1</v>
       </c>
@@ -3785,10 +3975,10 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3798,14 +3988,14 @@
         <v>1</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N48" s="6">
         <v>15.33</v>
@@ -3823,8 +4013,12 @@
         <f t="shared" si="2"/>
         <v>1,HM975-ND</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S48" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1,HM975-ND</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="4"/>
@@ -3846,8 +4040,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S49" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="4" t="s">
@@ -3873,17 +4071,21 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S50" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>1</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>83</v>
@@ -3915,8 +4117,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S51" s="4"/>
+    </row>
+    <row r="52" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>1</v>
       </c>
@@ -3947,7 +4150,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="4"/>

</xml_diff>

<commit_message>
Added Mouser parts reference and prices
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/v0.4_bom.xlsx
+++ b/reference/hardware/v0.4/v0.4_bom.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="265">
   <si>
     <t>Value</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Digikey P/N</t>
   </si>
   <si>
-    <t>Each</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -690,12 +687,6 @@
     <t>Board Reference 2 Channel</t>
   </si>
   <si>
-    <t>CTM Full</t>
-  </si>
-  <si>
-    <t>CTM 2 Ch</t>
-  </si>
-  <si>
     <t>HM975-ND</t>
   </si>
   <si>
@@ -751,6 +742,141 @@
   </si>
   <si>
     <t>2Ch Digikey import</t>
+  </si>
+  <si>
+    <t>Mouser Full</t>
+  </si>
+  <si>
+    <t>Mouser P/N</t>
+  </si>
+  <si>
+    <t>Digikey Price (USD)</t>
+  </si>
+  <si>
+    <t>Mouser Price (USD)</t>
+  </si>
+  <si>
+    <t>MPX4250AP</t>
+  </si>
+  <si>
+    <t>841-MPX4250AP</t>
+  </si>
+  <si>
+    <t>579-TC4424EPA</t>
+  </si>
+  <si>
+    <t>511-ULN2803A</t>
+  </si>
+  <si>
+    <t>ULN2803A</t>
+  </si>
+  <si>
+    <t>80-T356G106K035AT</t>
+  </si>
+  <si>
+    <t>80-C322C224K5R</t>
+  </si>
+  <si>
+    <t>80-C322C104M5R-TR</t>
+  </si>
+  <si>
+    <t>80-T356F476K6AT</t>
+  </si>
+  <si>
+    <t>581-AR215F334K4R</t>
+  </si>
+  <si>
+    <t>80-C317C103K5R</t>
+  </si>
+  <si>
+    <t>80-C330C105M5U</t>
+  </si>
+  <si>
+    <t>80-C317C472K1R</t>
+  </si>
+  <si>
+    <t>863-1N5919BG</t>
+  </si>
+  <si>
+    <t>833-1N5818-TP</t>
+  </si>
+  <si>
+    <t>833-1N4004-TP</t>
+  </si>
+  <si>
+    <t>667-ERZ-V14D220</t>
+  </si>
+  <si>
+    <t>511-STP62NS04Z</t>
+  </si>
+  <si>
+    <t>756-RC55Y-2K49BI</t>
+  </si>
+  <si>
+    <t>926-LM2940T-5.0/NOPB</t>
+  </si>
+  <si>
+    <t>517-9691020000DA</t>
+  </si>
+  <si>
+    <t>969102-0000-DA</t>
+  </si>
+  <si>
+    <t>571-5103308-8</t>
+  </si>
+  <si>
+    <t>71-RN60D-F-10K</t>
+  </si>
+  <si>
+    <t>71-RN60D-F-1.0K</t>
+  </si>
+  <si>
+    <t>279-LR1F680R</t>
+  </si>
+  <si>
+    <t>279-LR1F470R</t>
+  </si>
+  <si>
+    <t>279-H83K9BDA</t>
+  </si>
+  <si>
+    <t>279-YR1B1K0CC</t>
+  </si>
+  <si>
+    <t>603-MFR-25FBF52-100K</t>
+  </si>
+  <si>
+    <t>594-5083NW160R0J</t>
+  </si>
+  <si>
+    <t>CTM Full Digikey</t>
+  </si>
+  <si>
+    <t>CTM Full Mouser</t>
+  </si>
+  <si>
+    <t>859-LTL-4221N</t>
+  </si>
+  <si>
+    <t>546-1455N1202</t>
+  </si>
+  <si>
+    <t>571-1-2199298-2</t>
+  </si>
+  <si>
+    <t>571-2828362</t>
+  </si>
+  <si>
+    <t>782-A000026</t>
+  </si>
+  <si>
+    <t>Mouser price is crazy</t>
+  </si>
+  <si>
+    <t>CTM 2 Ch Digikey</t>
+  </si>
+  <si>
+    <t>CTM 2 Ch Mouser</t>
   </si>
 </sst>
 </file>
@@ -760,7 +886,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -821,8 +947,13 @@
       <color rgb="FFFF0000"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +988,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -977,7 +1114,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1053,11 +1190,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1451,10 +1598,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N31" workbookViewId="0">
-      <selection activeCell="S52" sqref="S52"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,24 +1612,25 @@
     <col min="6" max="6" width="53.1640625" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="12" max="12" width="17.1640625" customWidth="1"/>
-    <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="17" max="17" width="47.83203125" customWidth="1"/>
-    <col min="18" max="19" width="27.33203125" customWidth="1"/>
-    <col min="20" max="20" width="28" customWidth="1"/>
+    <col min="13" max="14" width="28" customWidth="1"/>
+    <col min="21" max="21" width="47.83203125" customWidth="1"/>
+    <col min="22" max="23" width="27.33203125" customWidth="1"/>
+    <col min="24" max="24" width="28" customWidth="1"/>
+    <col min="25" max="25" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1494,7 +1642,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1503,7 +1651,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1512,28 +1660,43 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="T1" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V1" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="4"/>
@@ -1550,21 +1713,25 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4" t="str">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="str">
         <f>IF(NOT(M2=""),A2&amp;","&amp;M2,"")</f>
         <v/>
       </c>
-      <c r="S2" s="4" t="str">
-        <f>IF(NOT(N2=""),B2&amp;","&amp;N2,"")</f>
+      <c r="W2" s="4" t="str">
+        <f>IF(NOT(O2=""),B2&amp;","&amp;O2,"")</f>
         <v/>
       </c>
-      <c r="T2" t="str">
+      <c r="X2" t="str">
         <f>A2&amp;"x "&amp;E2</f>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <f>LEN(C3)-LEN(SUBSTITUTE(C3,",",""))+1</f>
         <v>1</v>
@@ -1574,62 +1741,80 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3">
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="N3" s="5">
+      <c r="N3" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="O3" s="5">
         <v>1.7</v>
       </c>
-      <c r="O3" s="6">
-        <f t="shared" ref="O3:O10" si="1">N3*A3</f>
+      <c r="P3" s="5">
         <v>1.7</v>
       </c>
-      <c r="P3" s="6">
-        <f>N3*B3</f>
+      <c r="Q3" s="6">
+        <f t="shared" ref="Q3:Q10" si="1">O3*A3</f>
         <v>1.7</v>
       </c>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4" t="str">
-        <f t="shared" ref="R3:S51" si="2">IF(NOT(M3=""),A3&amp;","&amp;M3,"")</f>
+      <c r="R3" s="6">
+        <f>P3*A3</f>
+        <v>1.7</v>
+      </c>
+      <c r="S3" s="6">
+        <f>O3*B3</f>
+        <v>1.7</v>
+      </c>
+      <c r="T3" s="6">
+        <f>P3*B3</f>
+        <v>1.7</v>
+      </c>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4" t="str">
+        <f>IF(NOT(M3=""),A3&amp;","&amp;M3,"")</f>
         <v>1,399-3654-ND</v>
       </c>
-      <c r="S3" s="4" t="str">
+      <c r="W3" s="4" t="str">
         <f>IF(NOT(M3=""),B3&amp;","&amp;M3,"")</f>
         <v>1,399-3654-ND</v>
       </c>
-      <c r="T3" t="str">
+      <c r="X3" t="str">
         <f>"Capacitor - " &amp;A3&amp;"x "&amp;E3</f>
         <v>Capacitor - 1x 10uF</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y3" t="str">
+        <f>IF(NOT(L3=""),L3&amp;"|"&amp;A3,"")</f>
+        <v>T356G106K035AT|1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>LEN(C4)-LEN(SUBSTITUTE(C4,",",""))+1</f>
         <v>5</v>
@@ -1639,62 +1824,80 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3">
         <v>15</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="N4" s="5">
+        <v>179</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="O4" s="5">
         <v>0.66</v>
       </c>
-      <c r="O4" s="6">
+      <c r="P4" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="Q4" s="6">
         <f t="shared" si="1"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" ref="P4:P48" si="3">N4*B4</f>
+      <c r="R4" s="6">
+        <f t="shared" ref="R4:R51" si="2">P4*A4</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="S4" s="6">
+        <f>O4*B4</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="T4" s="6">
+        <f t="shared" ref="T4:T48" si="3">P4*B4</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4" t="str">
+        <f>IF(NOT(M4=""),A4&amp;","&amp;M4,"")</f>
         <v>5,399-4353-ND</v>
       </c>
-      <c r="S4" s="4" t="str">
-        <f t="shared" ref="S4:S48" si="4">IF(NOT(M4=""),B4&amp;","&amp;M4,"")</f>
+      <c r="W4" s="4" t="str">
+        <f t="shared" ref="W4:W48" si="4">IF(NOT(M4=""),B4&amp;","&amp;M4,"")</f>
         <v>5,399-4353-ND</v>
       </c>
-      <c r="T4" t="str">
-        <f t="shared" ref="T4:T10" si="5">"Capacitor - " &amp;A4&amp;"x "&amp;E4</f>
+      <c r="X4" t="str">
+        <f t="shared" ref="X4:X10" si="5">"Capacitor - " &amp;A4&amp;"x "&amp;E4</f>
         <v>Capacitor - 5x 0.22uF</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y4" t="str">
+        <f t="shared" ref="Y4:Y48" si="6">IF(NOT(L4=""),L4&amp;"|"&amp;A4,"")</f>
+        <v>C322C224K5R5TA|5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f>LEN(C5)-LEN(SUBSTITUTE(C5,",",""))+1</f>
         <v>7</v>
@@ -1704,62 +1907,80 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3">
         <v>17</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="O5" s="5">
         <v>0.32</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="Q5" s="6">
         <f t="shared" si="1"/>
         <v>2.2400000000000002</v>
       </c>
-      <c r="P5" s="6">
+      <c r="R5" s="6">
+        <f t="shared" si="2"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="S5" s="6">
+        <f>O5*B5</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="T5" s="6">
         <f t="shared" si="3"/>
         <v>2.2400000000000002</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4" t="str">
+        <f>IF(NOT(M5=""),A5&amp;","&amp;M5,"")</f>
         <v>7,399-9879-1-ND</v>
       </c>
-      <c r="S5" s="4" t="str">
+      <c r="W5" s="4" t="str">
         <f t="shared" si="4"/>
         <v>7,399-9879-1-ND</v>
       </c>
-      <c r="T5" t="str">
+      <c r="X5" t="str">
         <f t="shared" si="5"/>
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y5" t="str">
+        <f t="shared" si="6"/>
+        <v>C322C104M5R5TA7301|7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f>LEN(C6)-LEN(SUBSTITUTE(C6,",",""))+1</f>
         <v>1</v>
@@ -1769,64 +1990,82 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3">
         <v>2</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O6" s="5">
         <v>1.57</v>
       </c>
-      <c r="O6" s="6">
+      <c r="P6" s="5">
+        <v>1.57</v>
+      </c>
+      <c r="Q6" s="6">
         <f t="shared" si="1"/>
         <v>1.57</v>
       </c>
-      <c r="P6" s="6">
+      <c r="R6" s="6">
+        <f t="shared" si="2"/>
+        <v>1.57</v>
+      </c>
+      <c r="S6" s="6">
+        <f>O6*B6</f>
+        <v>1.57</v>
+      </c>
+      <c r="T6" s="6">
         <f t="shared" si="3"/>
         <v>1.57</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4" t="str">
+        <f>IF(NOT(M6=""),A6&amp;","&amp;M6,"")</f>
         <v>1,399-3652-ND</v>
       </c>
-      <c r="S6" s="4" t="str">
+      <c r="W6" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,399-3652-ND</v>
       </c>
-      <c r="T6" t="str">
+      <c r="X6" t="str">
         <f t="shared" si="5"/>
         <v>Capacitor - 1x 47uF</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y6" t="str">
+        <f t="shared" si="6"/>
+        <v>T356F476K006AT|1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
-        <f t="shared" ref="A7:A9" si="6">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
+        <f t="shared" ref="A7:A9" si="7">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B7" s="20">
@@ -1834,64 +2073,82 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3">
         <v>2</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="O7" s="5">
         <v>0.62</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="5">
+        <v>0.43</v>
+      </c>
+      <c r="Q7" s="6">
         <f t="shared" si="1"/>
         <v>0.62</v>
       </c>
-      <c r="P7" s="6">
+      <c r="R7" s="6">
+        <f t="shared" si="2"/>
+        <v>0.43</v>
+      </c>
+      <c r="S7" s="6">
+        <f>O7*B7</f>
+        <v>0.62</v>
+      </c>
+      <c r="T7" s="6">
         <f t="shared" si="3"/>
-        <v>0.62</v>
-      </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.43</v>
+      </c>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4" t="str">
+        <f>IF(NOT(M7=""),A7&amp;","&amp;M7,"")</f>
         <v>1,478-5120-ND</v>
       </c>
-      <c r="S7" s="4" t="str">
+      <c r="W7" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,478-5120-ND</v>
       </c>
-      <c r="T7" t="str">
+      <c r="X7" t="str">
         <f t="shared" si="5"/>
         <v>Capacitor - 1x 0.33uF</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y7" t="str">
+        <f t="shared" si="6"/>
+        <v>AR215F334K4R|1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="B8" s="20">
@@ -1899,64 +2156,82 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
         <v>3</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="O8" s="5">
         <v>0.24</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="Q8" s="6">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="P8" s="6">
+      <c r="R8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.24</v>
+      </c>
+      <c r="S8" s="6">
+        <f>O8*B8</f>
+        <v>0.24</v>
+      </c>
+      <c r="T8" s="6">
         <f t="shared" si="3"/>
         <v>0.24</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4" t="str">
+        <f>IF(NOT(M8=""),A8&amp;","&amp;M8,"")</f>
         <v>1,399-4206-ND</v>
       </c>
-      <c r="S8" s="4" t="str">
+      <c r="W8" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,399-4206-ND</v>
       </c>
-      <c r="T8" t="str">
+      <c r="X8" t="str">
         <f t="shared" si="5"/>
         <v>Capacitor - 1x 0.01uF</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y8" t="str">
+        <f t="shared" si="6"/>
+        <v>C317C103K5R5TA|1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="B9" s="20">
@@ -1964,62 +2239,80 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3">
         <v>4</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="O9" s="5">
         <v>0.66</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="Q9" s="6">
         <f t="shared" si="1"/>
         <v>1.98</v>
       </c>
-      <c r="P9" s="6">
+      <c r="R9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.98</v>
+      </c>
+      <c r="S9" s="6">
+        <f>O9*B9</f>
+        <v>1.32</v>
+      </c>
+      <c r="T9" s="6">
         <f t="shared" si="3"/>
         <v>1.32</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4" t="str">
+        <f>IF(NOT(M9=""),A9&amp;","&amp;M9,"")</f>
         <v>3,399-4390-ND</v>
       </c>
-      <c r="S9" s="4" t="str">
+      <c r="W9" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2,399-4390-ND</v>
       </c>
-      <c r="T9" t="str">
+      <c r="X9" t="str">
         <f t="shared" si="5"/>
         <v>Capacitor - 3x 1uF</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y9" t="str">
+        <f t="shared" si="6"/>
+        <v>C330C105M5U5TA|3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f>LEN(C10)-LEN(SUBSTITUTE(C10,",",""))+1</f>
         <v>1</v>
@@ -2029,60 +2322,78 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N10" s="5">
+        <v>139</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O10" s="5">
         <v>0.25</v>
       </c>
-      <c r="O10" s="6">
+      <c r="P10" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="Q10" s="6">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="P10" s="6">
+      <c r="R10" s="6">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="S10" s="6">
+        <f>O10*B10</f>
+        <v>0.25</v>
+      </c>
+      <c r="T10" s="6">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4" t="str">
+        <f>IF(NOT(M10=""),A10&amp;","&amp;M10,"")</f>
         <v>1,399-4243-ND</v>
       </c>
-      <c r="S10" s="4" t="str">
+      <c r="W10" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,399-4243-ND</v>
       </c>
-      <c r="T10" t="str">
+      <c r="X10" t="str">
         <f t="shared" si="5"/>
         <v>Capacitor - 1x 4.7nF</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y10" t="str">
+        <f t="shared" si="6"/>
+        <v>C317C472K1R5TA|1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="4"/>
@@ -2096,23 +2407,28 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
+      <c r="N11" s="2"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4" t="str">
+        <f>IF(NOT(M11=""),A11&amp;","&amp;M11,"")</f>
         <v/>
       </c>
-      <c r="S11" s="4" t="str">
+      <c r="W11" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="4"/>
@@ -2126,277 +2442,354 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="2"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4" t="str">
+        <f>IF(NOT(M12=""),A12&amp;","&amp;M12,"")</f>
         <v/>
       </c>
-      <c r="S12" s="4" t="str">
+      <c r="W12" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <f>LEN(C13)-LEN(SUBSTITUTE(C13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B13" s="20">
-        <f t="shared" ref="B13:B16" si="7">LEN(D13)-LEN(SUBSTITUTE(D13,",",""))+1</f>
+        <f t="shared" ref="B13:B16" si="8">LEN(D13)-LEN(SUBSTITUTE(D13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3">
         <v>1</v>
       </c>
       <c r="J13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L13" s="7" t="s">
+      <c r="M13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" s="5">
+      <c r="N13" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="O13" s="5">
         <v>0.34</v>
       </c>
-      <c r="O13" s="6">
-        <f>N13*A13</f>
+      <c r="P13" s="5">
+        <v>0.43</v>
+      </c>
+      <c r="Q13" s="6">
+        <f>O13*A13</f>
         <v>0.34</v>
       </c>
-      <c r="P13" s="6">
+      <c r="R13" s="6">
+        <f t="shared" si="2"/>
+        <v>0.43</v>
+      </c>
+      <c r="S13" s="6">
+        <f>O13*B13</f>
+        <v>0.34</v>
+      </c>
+      <c r="T13" s="6">
         <f t="shared" si="3"/>
-        <v>0.34</v>
-      </c>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.43</v>
+      </c>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4" t="str">
+        <f>IF(NOT(M13=""),A13&amp;","&amp;M13,"")</f>
         <v>1,1N5919BGOS-ND</v>
       </c>
-      <c r="S13" s="4" t="str">
+      <c r="W13" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,1N5919BGOS-ND</v>
       </c>
-      <c r="T13" t="str">
+      <c r="X13" t="str">
         <f>"Diode - " &amp;A13&amp;"x "&amp;E13</f>
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y13" t="str">
+        <f t="shared" si="6"/>
+        <v>1N5919BG|1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <f>LEN(C14)-LEN(SUBSTITUTE(C14,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B14" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3">
         <v>18</v>
       </c>
       <c r="J14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="5">
+      <c r="N14" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="O14" s="5">
         <v>0.39</v>
       </c>
-      <c r="O14" s="6">
-        <f>N14*A14</f>
+      <c r="P14" s="5">
+        <v>0.39</v>
+      </c>
+      <c r="Q14" s="6">
+        <f>O14*A14</f>
         <v>4.68</v>
       </c>
-      <c r="P14" s="6">
+      <c r="R14" s="6">
+        <f t="shared" si="2"/>
+        <v>4.68</v>
+      </c>
+      <c r="S14" s="6">
+        <f>O14*B14</f>
+        <v>4.68</v>
+      </c>
+      <c r="T14" s="6">
         <f t="shared" si="3"/>
         <v>4.68</v>
       </c>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4" t="str">
+        <f>IF(NOT(M14=""),A14&amp;","&amp;M14,"")</f>
         <v>12,1N5818-TPCT-ND</v>
       </c>
-      <c r="S14" s="4" t="str">
+      <c r="W14" s="4" t="str">
         <f t="shared" si="4"/>
         <v>12,1N5818-TPCT-ND</v>
       </c>
-      <c r="T14" t="str">
-        <f t="shared" ref="T14:T16" si="8">"Diode - " &amp;A14&amp;"x "&amp;E14</f>
+      <c r="X14" t="str">
+        <f t="shared" ref="X14:X16" si="9">"Diode - " &amp;A14&amp;"x "&amp;E14</f>
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y14" t="str">
+        <f t="shared" si="6"/>
+        <v>1N5818-TP|12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <f>LEN(C15)-LEN(SUBSTITUTE(C15,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B15" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="N15" s="5">
+        <v>119</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="O15" s="5">
         <v>0.47</v>
       </c>
-      <c r="O15" s="6">
-        <f>N15*A15</f>
+      <c r="P15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="Q15" s="6">
+        <f>O15*A15</f>
         <v>3.76</v>
       </c>
-      <c r="P15" s="6">
+      <c r="R15" s="6">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="S15" s="6">
+        <f>O15*B15</f>
+        <v>1.88</v>
+      </c>
+      <c r="T15" s="6">
         <f t="shared" si="3"/>
-        <v>1.88</v>
-      </c>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4" t="str">
+        <f>IF(NOT(M15=""),A15&amp;","&amp;M15,"")</f>
         <v>8,160-1139-ND</v>
       </c>
-      <c r="S15" s="4" t="str">
+      <c r="W15" s="4" t="str">
         <f t="shared" si="4"/>
         <v>4,160-1139-ND</v>
       </c>
-      <c r="T15" t="str">
-        <f t="shared" si="8"/>
+      <c r="X15" t="str">
+        <f t="shared" si="9"/>
         <v>Diode - 8x LED-Red</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y15" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <f>LEN(C16)-LEN(SUBSTITUTE(C16,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B16" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
         <v>13</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N16" s="5">
+      <c r="N16" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="O16" s="5">
         <v>0.11</v>
       </c>
-      <c r="O16" s="6">
-        <f>N16*A16</f>
+      <c r="P16" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="Q16" s="6">
+        <f>O16*A16</f>
         <v>0.44</v>
       </c>
-      <c r="P16" s="6">
+      <c r="R16" s="6">
+        <f t="shared" si="2"/>
+        <v>0.44</v>
+      </c>
+      <c r="S16" s="6">
+        <f>O16*B16</f>
+        <v>0.22</v>
+      </c>
+      <c r="T16" s="6">
         <f t="shared" si="3"/>
         <v>0.22</v>
       </c>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4" t="str">
+        <f>IF(NOT(M16=""),A16&amp;","&amp;M16,"")</f>
         <v>4,1N4004-TPMSCT-ND</v>
       </c>
-      <c r="S16" s="4" t="str">
+      <c r="W16" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2,1N4004-TPMSCT-ND</v>
       </c>
-      <c r="T16" t="str">
-        <f t="shared" si="8"/>
+      <c r="X16" t="str">
+        <f t="shared" si="9"/>
         <v>Diode - 4x 1N4004</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y16" t="str">
+        <f t="shared" si="6"/>
+        <v>1N4004-TP|4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="4"/>
@@ -2410,27 +2803,32 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
+      <c r="N17" s="2"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4" t="str">
+        <f>IF(NOT(M17=""),A17&amp;","&amp;M17,"")</f>
         <v/>
       </c>
-      <c r="S17" s="4" t="str">
+      <c r="W17" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="T17" t="str">
-        <f t="shared" ref="T17:T46" si="9">A17&amp;"x "&amp;E17</f>
+      <c r="X17" t="str">
+        <f t="shared" ref="X17:X46" si="10">A17&amp;"x "&amp;E17</f>
         <v xml:space="preserve">x </v>
       </c>
-    </row>
-    <row r="18" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="4"/>
@@ -2444,27 +2842,32 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
       <c r="Q18" s="3"/>
-      <c r="R18" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="4" t="str">
+        <f>IF(NOT(M18=""),A18&amp;","&amp;M18,"")</f>
         <v/>
       </c>
-      <c r="S18" s="4" t="str">
+      <c r="W18" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="T18" t="str">
-        <f t="shared" si="9"/>
+      <c r="X18" t="str">
+        <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y18" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="4"/>
@@ -2478,91 +2881,114 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
+      <c r="N19" s="2"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4" t="str">
+        <f>IF(NOT(M19=""),A19&amp;","&amp;M19,"")</f>
         <v/>
       </c>
-      <c r="S19" s="4" t="str">
+      <c r="W19" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="T19" t="str">
-        <f t="shared" si="9"/>
+      <c r="X19" t="str">
+        <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
-    </row>
-    <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y19" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>1</v>
       </c>
       <c r="B20" s="20">
-        <f t="shared" ref="B20" si="10">LEN(D20)-LEN(SUBSTITUTE(D20,",",""))+1</f>
+        <f t="shared" ref="B20" si="11">LEN(D20)-LEN(SUBSTITUTE(D20,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3">
         <v>1</v>
       </c>
       <c r="J20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N20" s="5">
+      <c r="N20" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="O20" s="5">
         <v>0.72</v>
       </c>
-      <c r="O20" s="6">
-        <f>N20*A20</f>
+      <c r="P20" s="5">
         <v>0.72</v>
       </c>
-      <c r="P20" s="6">
+      <c r="Q20" s="6">
+        <f>O20*A20</f>
+        <v>0.72</v>
+      </c>
+      <c r="R20" s="6">
+        <f t="shared" si="2"/>
+        <v>0.72</v>
+      </c>
+      <c r="S20" s="6">
+        <f>O20*B20</f>
+        <v>0.72</v>
+      </c>
+      <c r="T20" s="6">
         <f t="shared" si="3"/>
         <v>0.72</v>
       </c>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4" t="str">
+        <f>IF(NOT(M20=""),A20&amp;","&amp;M20,"")</f>
         <v>1,P7307-ND</v>
       </c>
-      <c r="S20" s="4" t="str">
+      <c r="W20" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,P7307-ND</v>
       </c>
-      <c r="T20" t="str">
-        <f t="shared" si="9"/>
+      <c r="X20" t="str">
+        <f t="shared" si="10"/>
         <v>1x Surge Protection</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y20" t="str">
+        <f t="shared" si="6"/>
+        <v>ERZ-V14D220|1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="4"/>
@@ -2576,89 +3002,118 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
+      <c r="N21" s="2"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="6">
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6">
+        <f>O21*B21</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4" t="str">
+        <f>IF(NOT(M21=""),A21&amp;","&amp;M21,"")</f>
         <v/>
       </c>
-      <c r="S21" s="4" t="str">
+      <c r="W21" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="T21" t="str">
-        <f t="shared" si="9"/>
+      <c r="X21" t="str">
+        <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
-    </row>
-    <row r="22" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>1</v>
       </c>
       <c r="B22" s="20">
-        <f t="shared" ref="B22" si="11">LEN(D22)-LEN(SUBSTITUTE(D22,",",""))+1</f>
+        <f t="shared" ref="B22" si="12">LEN(D22)-LEN(SUBSTITUTE(D22,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="Q22" s="6">
+        <f>O22*A22</f>
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="R22" s="6">
+        <f t="shared" si="2"/>
+        <v>0.51</v>
+      </c>
+      <c r="S22" s="6">
+        <f>O22*B22</f>
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="T22" s="6">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+      <c r="U22" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="M22" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N22" s="3">
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="O22" s="6">
-        <f>N22*A22</f>
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="P22" s="6">
-        <f t="shared" si="3"/>
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="R22" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="V22" s="4" t="str">
+        <f>IF(NOT(M22=""),A22&amp;","&amp;M22,"")</f>
         <v>1,ED2561-ND</v>
       </c>
-      <c r="S22" s="4" t="str">
+      <c r="W22" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,ED2561-ND</v>
       </c>
-      <c r="T22" t="str">
+      <c r="X22" t="str">
         <f>A22&amp;"x "&amp;E22</f>
         <v>1x Dual Terminal Block</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y22" t="str">
+        <f t="shared" si="6"/>
+        <v>OSTTA020161|1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>5</v>
       </c>
@@ -2666,54 +3121,74 @@
         <v>5</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L23" s="3"/>
+        <v>196</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="M23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="N23" s="5">
+        <v>109</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="O23" s="5">
         <v>0.1</v>
       </c>
-      <c r="O23" s="6">
-        <f>N23*A23</f>
+      <c r="P23" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="Q23" s="6">
+        <f>O23*A23</f>
         <v>0.5</v>
       </c>
-      <c r="P23" s="6">
+      <c r="R23" s="6">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="S23" s="6">
+        <f>O23*B23</f>
+        <v>0.5</v>
+      </c>
+      <c r="T23" s="6">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4" t="str">
+        <f>IF(NOT(M23=""),A23&amp;","&amp;M23,"")</f>
         <v>5,3M9580-ND</v>
       </c>
-      <c r="S23" s="4" t="str">
+      <c r="W23" s="4" t="str">
         <f t="shared" si="4"/>
         <v>5,3M9580-ND</v>
       </c>
-      <c r="T23" t="str">
-        <f t="shared" si="9"/>
+      <c r="X23" t="str">
+        <f t="shared" si="10"/>
         <v>5x Jumper</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y23" t="str">
+        <f t="shared" si="6"/>
+        <v>969102-0000-DA|5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>2</v>
       </c>
@@ -2721,16 +3196,16 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2738,43 +3213,63 @@
         <v>1</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N24" s="6">
+        <v>125</v>
+      </c>
+      <c r="N24" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="O24" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="O24" s="6">
-        <f>N24*A24</f>
+      <c r="P24" s="32">
+        <v>2.95</v>
+      </c>
+      <c r="Q24" s="6">
+        <f>O24*A24</f>
         <v>1.1200000000000001</v>
       </c>
-      <c r="P24" s="6">
+      <c r="R24" s="6">
+        <f t="shared" si="2"/>
+        <v>5.9</v>
+      </c>
+      <c r="S24" s="6">
+        <f>O24*B24</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="T24" s="6">
         <f t="shared" si="3"/>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>5.9</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="V24" s="4" t="str">
+        <f>IF(NOT(M24=""),A24&amp;","&amp;M24,"")</f>
         <v>2,S1012EC-40-ND</v>
       </c>
-      <c r="S24" s="4" t="str">
+      <c r="W24" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2,S1012EC-40-ND</v>
       </c>
-      <c r="T24" t="str">
-        <f t="shared" si="9"/>
+      <c r="X24" t="str">
+        <f t="shared" si="10"/>
         <v>2x 40 POS 0.100 Pin Header</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="53" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y24" t="str">
+        <f t="shared" si="6"/>
+        <v>PREC040SAAN-RC|2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>1</v>
       </c>
@@ -2782,16 +3277,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -2799,43 +3294,61 @@
         <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M25" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="N25" s="6">
+        <v>212</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="O25" s="6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="O25" s="6">
-        <f>N25*A25</f>
+      <c r="P25" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="6">
+        <f>O25*A25</f>
         <v>1.1299999999999999</v>
       </c>
-      <c r="P25" s="6">
-        <f t="shared" ref="P25" si="12">N25*B25</f>
+      <c r="R25" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="S25" s="6">
+        <f>O25*B25</f>
         <v>1.1299999999999999</v>
       </c>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4" t="str">
-        <f t="shared" ref="R25:S25" si="13">IF(NOT(M25=""),A25&amp;","&amp;M25,"")</f>
+      <c r="T25" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4" t="str">
+        <f t="shared" ref="V25" si="13">IF(NOT(M25=""),A25&amp;","&amp;M25,"")</f>
         <v>1,1175-1614-ND</v>
       </c>
-      <c r="S25" s="4" t="str">
+      <c r="W25" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,1175-1614-ND</v>
       </c>
-      <c r="T25" t="str">
-        <f t="shared" ref="T25" si="14">A25&amp;"x "&amp;E25</f>
+      <c r="X25" t="str">
+        <f t="shared" ref="X25" si="14">A25&amp;"x "&amp;E25</f>
         <v>1x Rectangular Connectors - Headers, Male Pins</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y25" t="str">
+        <f t="shared" si="6"/>
+        <v>3020-40-0100-00|1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="4"/>
@@ -2849,24 +3362,32 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4" t="str">
+        <f>IF(NOT(M26=""),A26&amp;","&amp;M26,"")</f>
         <v/>
       </c>
-      <c r="S26" s="4" t="str">
+      <c r="W26" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="T26" t="str">
-        <f t="shared" si="9"/>
+      <c r="X26" t="str">
+        <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
-    </row>
-    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y26" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="4"/>
@@ -2880,24 +3401,32 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4" t="str">
+        <f>IF(NOT(M27=""),A27&amp;","&amp;M27,"")</f>
         <v/>
       </c>
-      <c r="S27" s="4" t="str">
+      <c r="W27" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="T27" t="str">
-        <f t="shared" si="9"/>
+      <c r="X27" t="str">
+        <f t="shared" si="10"/>
         <v xml:space="preserve">x </v>
       </c>
-    </row>
-    <row r="28" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y27" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <f>LEN(C28)-LEN(SUBSTITUTE(C28,",",""))+1</f>
         <v>8</v>
@@ -2907,62 +3436,80 @@
         <v>6</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3">
         <v>8</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="N28" s="6">
+        <v>106</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="O28" s="6">
         <v>1.51</v>
       </c>
-      <c r="O28" s="6">
-        <f>N28*A28</f>
+      <c r="P28" s="6">
+        <v>1.51</v>
+      </c>
+      <c r="Q28" s="6">
+        <f>O28*A28</f>
         <v>12.08</v>
       </c>
-      <c r="P28" s="6">
+      <c r="R28" s="6">
+        <f t="shared" si="2"/>
+        <v>12.08</v>
+      </c>
+      <c r="S28" s="6">
+        <f>O28*B28</f>
+        <v>9.06</v>
+      </c>
+      <c r="T28" s="6">
         <f t="shared" si="3"/>
         <v>9.06</v>
       </c>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4" t="str">
+        <f>IF(NOT(M28=""),A28&amp;","&amp;M28,"")</f>
         <v>8,497-5896-5-ND</v>
       </c>
-      <c r="S28" s="4" t="str">
+      <c r="W28" s="4" t="str">
         <f>IF(NOT(M28=""),B28&amp;","&amp;M28,"")</f>
         <v>6,497-5896-5-ND</v>
       </c>
-      <c r="T28" t="str">
-        <f t="shared" si="9"/>
+      <c r="X28" t="str">
+        <f t="shared" si="10"/>
         <v>8x 62A MOSFET N-CH</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y28" t="str">
+        <f t="shared" si="6"/>
+        <v>STP62NS04Z|8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="4"/>
@@ -2976,20 +3523,28 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="3"/>
+      <c r="N29" s="2"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4" t="str">
+        <f>IF(NOT(M29=""),A29&amp;","&amp;M29,"")</f>
         <v/>
       </c>
-      <c r="S29" s="4" t="str">
+      <c r="W29" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y29" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="4"/>
@@ -3003,20 +3558,28 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="3"/>
+      <c r="N30" s="2"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4" t="str">
+        <f>IF(NOT(M30=""),A30&amp;","&amp;M30,"")</f>
         <v/>
       </c>
-      <c r="S30" s="4" t="str">
+      <c r="W30" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y30" t="str">
+        <f>IF(NOT(L30=""),L30&amp;"|"&amp;A30,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <f>LEN(C31)-LEN(SUBSTITUTE(C31,",",""))+1</f>
         <v>5</v>
@@ -3026,16 +3589,16 @@
         <v>5</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -3043,43 +3606,61 @@
         <v>7</v>
       </c>
       <c r="J31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L31" s="3" t="s">
+      <c r="M31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N31" s="5">
+      <c r="N31" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="O31" s="5">
         <v>0.08</v>
       </c>
-      <c r="O31" s="6">
-        <f t="shared" ref="O31:O39" si="17">N31*A31</f>
+      <c r="P31" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="Q31" s="6">
+        <f t="shared" ref="Q31:Q39" si="17">O31*A31</f>
         <v>0.4</v>
       </c>
-      <c r="P31" s="6">
+      <c r="R31" s="6">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S31" s="6">
+        <f>O31*B31</f>
+        <v>0.4</v>
+      </c>
+      <c r="T31" s="6">
         <f t="shared" si="3"/>
-        <v>0.4</v>
-      </c>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4" t="str">
+        <f>IF(NOT(M31=""),A31&amp;","&amp;M31,"")</f>
         <v>5,10.0KXBK-ND</v>
       </c>
-      <c r="S31" s="4" t="str">
+      <c r="W31" s="4" t="str">
         <f t="shared" si="4"/>
         <v>5,10.0KXBK-ND</v>
       </c>
-      <c r="T31" t="str">
+      <c r="X31" t="str">
         <f>"Resistor - " &amp; A31&amp;"x "&amp;E31</f>
         <v>Resistor - 5x 10k</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y31" t="str">
+        <f t="shared" si="6"/>
+        <v>MFR-25FBF-10K0|5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <f>LEN(C32)-LEN(SUBSTITUTE(C32,",",""))+1</f>
         <v>12</v>
@@ -3089,16 +3670,16 @@
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -3106,43 +3687,61 @@
         <v>32</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N32" s="5">
+      <c r="N32" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="O32" s="5">
         <v>0.06</v>
       </c>
-      <c r="O32" s="6">
+      <c r="P32" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="Q32" s="6">
         <f t="shared" si="17"/>
         <v>0.72</v>
       </c>
-      <c r="P32" s="6">
+      <c r="R32" s="6">
+        <f t="shared" si="2"/>
+        <v>1.32</v>
+      </c>
+      <c r="S32" s="6">
+        <f>O32*B32</f>
+        <v>0.48</v>
+      </c>
+      <c r="T32" s="6">
         <f t="shared" si="3"/>
-        <v>0.48</v>
-      </c>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.88</v>
+      </c>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4" t="str">
+        <f>IF(NOT(M32=""),A32&amp;","&amp;M32,"")</f>
         <v>12,1.00KXBK-ND</v>
       </c>
-      <c r="S32" s="4" t="str">
+      <c r="W32" s="4" t="str">
         <f t="shared" si="4"/>
         <v>8,1.00KXBK-ND</v>
       </c>
-      <c r="T32" t="str">
-        <f t="shared" ref="T32:T39" si="18">"Resistor - " &amp; A32&amp;"x "&amp;E32</f>
+      <c r="X32" t="str">
+        <f t="shared" ref="X32:X39" si="18">"Resistor - " &amp; A32&amp;"x "&amp;E32</f>
         <v>Resistor - 12x 1k</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y32" t="str">
+        <f t="shared" si="6"/>
+        <v>MFR-25FBF-1K00|12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <f>LEN(C33)-LEN(SUBSTITUTE(C33,",",""))+1</f>
         <v>8</v>
@@ -3152,58 +3751,76 @@
         <v>4</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E33" s="13">
         <v>680</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L33" s="7"/>
       <c r="M33" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="N33" s="14">
+        <v>169</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="O33" s="14">
         <v>0.22</v>
       </c>
-      <c r="O33" s="6">
+      <c r="P33" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="Q33" s="6">
         <f t="shared" si="17"/>
         <v>1.76</v>
       </c>
-      <c r="P33" s="6">
+      <c r="R33" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="S33" s="6">
+        <f>O33*B33</f>
+        <v>0.88</v>
+      </c>
+      <c r="T33" s="6">
         <f t="shared" si="3"/>
-        <v>0.88</v>
-      </c>
-      <c r="Q33" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="R33" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="U33" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="V33" s="4" t="str">
+        <f>IF(NOT(M33=""),A33&amp;","&amp;M33,"")</f>
         <v>8,A105963CT-ND</v>
       </c>
-      <c r="S33" s="4" t="str">
+      <c r="W33" s="4" t="str">
         <f t="shared" si="4"/>
         <v>4,A105963CT-ND</v>
       </c>
-      <c r="T33" t="str">
+      <c r="X33" t="str">
         <f t="shared" si="18"/>
         <v>Resistor - 8x 680</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <f>LEN(C34)-LEN(SUBSTITUTE(C34,",",""))+1</f>
         <v>6</v>
@@ -3213,16 +3830,16 @@
         <v>6</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E34" s="3">
         <v>470</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -3230,43 +3847,61 @@
         <v>9</v>
       </c>
       <c r="J34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L34" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L34" s="7" t="s">
+      <c r="M34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N34" s="5">
+      <c r="N34" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="O34" s="5">
         <v>0.11</v>
       </c>
-      <c r="O34" s="6">
+      <c r="P34" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="Q34" s="6">
         <f t="shared" si="17"/>
         <v>0.66</v>
       </c>
-      <c r="P34" s="6">
+      <c r="R34" s="6">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="S34" s="6">
+        <f>O34*B34</f>
+        <v>0.66</v>
+      </c>
+      <c r="T34" s="6">
         <f t="shared" si="3"/>
-        <v>0.66</v>
-      </c>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4" t="str">
+        <f>IF(NOT(M34=""),A34&amp;","&amp;M34,"")</f>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
-      <c r="S34" s="4" t="str">
+      <c r="W34" s="4" t="str">
         <f t="shared" si="4"/>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
-      <c r="T34" t="str">
+      <c r="X34" t="str">
         <f t="shared" si="18"/>
         <v>Resistor - 6x 470</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y34" t="str">
+        <f t="shared" si="6"/>
+        <v>RNF14FTD470R|6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>2</v>
       </c>
@@ -3275,62 +3910,80 @@
         <v>2</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
         <v>3</v>
       </c>
       <c r="J35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L35" s="3" t="s">
+      <c r="M35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N35" s="5">
+      <c r="N35" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O35" s="5">
         <v>1.92</v>
       </c>
-      <c r="O35" s="6">
+      <c r="P35" s="5">
+        <v>1.92</v>
+      </c>
+      <c r="Q35" s="6">
         <f t="shared" si="17"/>
         <v>3.84</v>
       </c>
-      <c r="P35" s="6">
+      <c r="R35" s="6">
+        <f t="shared" si="2"/>
+        <v>3.84</v>
+      </c>
+      <c r="S35" s="6">
+        <f>O35*B35</f>
+        <v>3.84</v>
+      </c>
+      <c r="T35" s="6">
         <f t="shared" si="3"/>
         <v>3.84</v>
       </c>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4" t="str">
+        <f>IF(NOT(M35=""),A35&amp;","&amp;M35,"")</f>
         <v>2,985-1047-1-ND</v>
       </c>
-      <c r="S35" s="4" t="str">
+      <c r="W35" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2,985-1047-1-ND</v>
       </c>
-      <c r="T35" t="str">
+      <c r="X35" t="str">
         <f t="shared" si="18"/>
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y35" t="str">
+        <f t="shared" si="6"/>
+        <v>RC55Y-2K49BI|2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>1</v>
       </c>
@@ -3339,16 +3992,16 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -3356,45 +4009,63 @@
         <v>1</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M36" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N36" s="5">
+      <c r="N36" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="O36" s="5">
         <v>0.46</v>
       </c>
-      <c r="O36" s="6">
+      <c r="P36" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q36" s="6">
         <f t="shared" si="17"/>
         <v>0.46</v>
       </c>
-      <c r="P36" s="6">
+      <c r="R36" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S36" s="6">
+        <f>O36*B36</f>
+        <v>0.46</v>
+      </c>
+      <c r="T36" s="6">
         <f t="shared" si="3"/>
-        <v>0.46</v>
-      </c>
-      <c r="Q36" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="R36" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U36" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="V36" s="4" t="str">
+        <f>IF(NOT(M36=""),A36&amp;","&amp;M36,"")</f>
         <v>1,3.9KADCT-ND</v>
       </c>
-      <c r="S36" s="4" t="str">
+      <c r="W36" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,3.9KADCT-ND</v>
       </c>
-      <c r="T36" t="str">
+      <c r="X36" t="str">
         <f t="shared" si="18"/>
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y36" t="str">
+        <f t="shared" si="6"/>
+        <v>MFP-25BRD52-3K9|1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>1</v>
       </c>
@@ -3403,16 +4074,16 @@
         <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -3420,45 +4091,63 @@
         <v>1</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M37" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N37" s="5">
+      <c r="N37" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="O37" s="5">
         <v>0.46</v>
       </c>
-      <c r="O37" s="6">
+      <c r="P37" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q37" s="6">
         <f t="shared" si="17"/>
         <v>0.46</v>
       </c>
-      <c r="P37" s="6">
+      <c r="R37" s="6">
+        <f t="shared" si="2"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S37" s="6">
+        <f>O37*B37</f>
+        <v>0.46</v>
+      </c>
+      <c r="T37" s="6">
         <f t="shared" si="3"/>
-        <v>0.46</v>
-      </c>
-      <c r="Q37" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="R37" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="V37" s="4" t="str">
+        <f>IF(NOT(M37=""),A37&amp;","&amp;M37,"")</f>
         <v>1,1KADCT-ND</v>
       </c>
-      <c r="S37" s="4" t="str">
+      <c r="W37" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,1KADCT-ND</v>
       </c>
-      <c r="T37" t="str">
+      <c r="X37" t="str">
         <f t="shared" si="18"/>
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y37" t="str">
+        <f t="shared" si="6"/>
+        <v>MFP-25BRD52-1K|1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <f t="shared" ref="A38:A39" si="19">LEN(C38)-LEN(SUBSTITUTE(C38,",",""))+1</f>
         <v>12</v>
@@ -3468,16 +4157,16 @@
         <v>8</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -3485,43 +4174,61 @@
         <v>17</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="M38" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N38" s="5">
+      <c r="N38" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="O38" s="5">
         <v>0.1</v>
       </c>
-      <c r="O38" s="6">
+      <c r="P38" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="Q38" s="6">
         <f t="shared" si="17"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="P38" s="6">
+      <c r="R38" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="S38" s="6">
+        <f>O38*B38</f>
+        <v>0.8</v>
+      </c>
+      <c r="T38" s="6">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4" t="str">
+        <f>IF(NOT(M38=""),A38&amp;","&amp;M38,"")</f>
         <v>12,100KXBK-ND</v>
       </c>
-      <c r="S38" s="4" t="str">
+      <c r="W38" s="4" t="str">
         <f t="shared" si="4"/>
         <v>8,100KXBK-ND</v>
       </c>
-      <c r="T38" t="str">
+      <c r="X38" t="str">
         <f t="shared" si="18"/>
         <v>Resistor - 12x 100k</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y38" t="str">
+        <f t="shared" si="6"/>
+        <v>MFR-25FBF-100K|12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <f t="shared" si="19"/>
         <v>4</v>
@@ -3531,16 +4238,16 @@
         <v>2</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E39" s="3">
         <v>160</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3548,43 +4255,61 @@
         <v>4</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M39" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N39" s="5">
+      <c r="N39" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="O39" s="5">
         <v>0.27</v>
       </c>
-      <c r="O39" s="6">
+      <c r="P39" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="Q39" s="6">
         <f t="shared" si="17"/>
         <v>1.08</v>
       </c>
-      <c r="P39" s="6">
+      <c r="R39" s="6">
+        <f t="shared" si="2"/>
+        <v>0.92</v>
+      </c>
+      <c r="S39" s="6">
+        <f>O39*B39</f>
+        <v>0.54</v>
+      </c>
+      <c r="T39" s="6">
         <f t="shared" si="3"/>
-        <v>0.54</v>
-      </c>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.46</v>
+      </c>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4" t="str">
+        <f>IF(NOT(M39=""),A39&amp;","&amp;M39,"")</f>
         <v>4,160YCT-ND</v>
       </c>
-      <c r="S39" s="4" t="str">
+      <c r="W39" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2,160YCT-ND</v>
       </c>
-      <c r="T39" t="str">
+      <c r="X39" t="str">
         <f t="shared" si="18"/>
         <v>Resistor - 4x 160</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y39" t="str">
+        <f t="shared" si="6"/>
+        <v>FMP200FRF52-160R|4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="4"/>
@@ -3598,20 +4323,28 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="2"/>
-      <c r="N40" s="3"/>
+      <c r="N40" s="2"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4" t="str">
+        <f>IF(NOT(M40=""),A40&amp;","&amp;M40,"")</f>
         <v/>
       </c>
-      <c r="S40" s="4" t="str">
+      <c r="W40" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y40" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="4"/>
@@ -3625,20 +4358,28 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="2"/>
-      <c r="N41" s="3"/>
+      <c r="N41" s="2"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4" t="str">
+        <f>IF(NOT(M41=""),A41&amp;","&amp;M41,"")</f>
         <v/>
       </c>
-      <c r="S41" s="4" t="str">
+      <c r="W41" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y41" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>1</v>
       </c>
@@ -3647,62 +4388,80 @@
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3">
         <v>2</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="N42" s="5">
+        <v>74</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="O42" s="5">
         <v>1.68</v>
       </c>
-      <c r="O42" s="6">
-        <f>N42*A42</f>
+      <c r="P42" s="5">
+        <v>1.67</v>
+      </c>
+      <c r="Q42" s="6">
+        <f>O42*A42</f>
         <v>1.68</v>
       </c>
-      <c r="P42" s="6">
+      <c r="R42" s="6">
+        <f t="shared" si="2"/>
+        <v>1.67</v>
+      </c>
+      <c r="S42" s="6">
+        <f>O42*B42</f>
+        <v>1.68</v>
+      </c>
+      <c r="T42" s="6">
         <f t="shared" si="3"/>
-        <v>1.68</v>
-      </c>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>1.67</v>
+      </c>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4" t="str">
+        <f>IF(NOT(M42=""),A42&amp;","&amp;M42,"")</f>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
-      <c r="S42" s="4" t="str">
+      <c r="W42" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
-      <c r="T42" t="str">
-        <f t="shared" si="9"/>
+      <c r="X42" t="str">
+        <f t="shared" si="10"/>
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y42" t="str">
+        <f t="shared" si="6"/>
+        <v>LM2940T-5.0/NOPB|1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>1</v>
       </c>
@@ -3711,58 +4470,78 @@
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3">
         <v>1</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
+      <c r="L43" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="M43" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N43" s="6">
+        <v>95</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O43" s="6">
         <v>15.41</v>
       </c>
-      <c r="O43" s="6">
-        <f>N43*A43</f>
+      <c r="P43" s="6">
+        <v>15.37</v>
+      </c>
+      <c r="Q43" s="6">
+        <f>O43*A43</f>
         <v>15.41</v>
       </c>
-      <c r="P43" s="6">
+      <c r="R43" s="6">
+        <f t="shared" si="2"/>
+        <v>15.37</v>
+      </c>
+      <c r="S43" s="6">
+        <f>O43*B43</f>
+        <v>15.41</v>
+      </c>
+      <c r="T43" s="6">
         <f t="shared" si="3"/>
-        <v>15.41</v>
-      </c>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>15.37</v>
+      </c>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4" t="str">
+        <f>IF(NOT(M43=""),A43&amp;","&amp;M43,"")</f>
         <v>1,MPX4250AP-ND</v>
       </c>
-      <c r="S43" s="4" t="str">
+      <c r="W43" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,MPX4250AP-ND</v>
       </c>
-      <c r="T43" t="str">
-        <f t="shared" si="9"/>
+      <c r="X43" t="str">
+        <f t="shared" si="10"/>
         <v>1x 1-Bar MAP sensor</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y43" t="str">
+        <f t="shared" si="6"/>
+        <v>MPX4250AP|1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>2</v>
       </c>
@@ -3771,60 +4550,80 @@
         <v>1</v>
       </c>
       <c r="C44" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="E44" s="13" t="s">
+      <c r="F44" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="G44" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="13">
         <v>2</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="L44" s="13"/>
+        <v>195</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>155</v>
+      </c>
       <c r="M44" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="N44" s="23">
+        <v>158</v>
+      </c>
+      <c r="N44" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="O44" s="23">
         <v>2.92</v>
       </c>
-      <c r="O44" s="6">
-        <f>N44*A44</f>
+      <c r="P44" s="23">
+        <v>2.92</v>
+      </c>
+      <c r="Q44" s="6">
+        <f>O44*A44</f>
         <v>5.84</v>
       </c>
-      <c r="P44" s="6">
+      <c r="R44" s="6">
+        <f t="shared" si="2"/>
+        <v>5.84</v>
+      </c>
+      <c r="S44" s="6">
+        <f>O44*B44</f>
+        <v>2.92</v>
+      </c>
+      <c r="T44" s="6">
         <f t="shared" si="3"/>
         <v>2.92</v>
       </c>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="4" t="str">
+        <f>IF(NOT(M44=""),A44&amp;","&amp;M44,"")</f>
         <v>2,TC4424EPA-ND</v>
       </c>
-      <c r="S44" s="4" t="str">
+      <c r="W44" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,TC4424EPA-ND</v>
       </c>
-      <c r="T44" t="str">
-        <f t="shared" si="9"/>
+      <c r="X44" t="str">
+        <f t="shared" si="10"/>
         <v>2x TC4424EPA</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y44" t="str">
+        <f t="shared" si="6"/>
+        <v>TC4424EPA|2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22">
         <v>1</v>
       </c>
@@ -3832,60 +4631,80 @@
         <v>1</v>
       </c>
       <c r="C45" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13">
         <v>1</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="L45" s="13"/>
+        <v>195</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>228</v>
+      </c>
       <c r="M45" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="N45" s="23">
+        <v>205</v>
+      </c>
+      <c r="N45" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="O45" s="23">
         <v>0.72</v>
       </c>
-      <c r="O45" s="6">
-        <f>N45*A45</f>
+      <c r="P45" s="23">
+        <v>0.92</v>
+      </c>
+      <c r="Q45" s="6">
+        <f>O45*A45</f>
         <v>0.72</v>
       </c>
-      <c r="P45" s="6">
-        <f t="shared" ref="P45" si="21">N45*B45</f>
+      <c r="R45" s="6">
+        <f t="shared" si="2"/>
+        <v>0.92</v>
+      </c>
+      <c r="S45" s="6">
+        <f>O45*B45</f>
         <v>0.72</v>
       </c>
-      <c r="Q45" s="12"/>
-      <c r="R45" s="4" t="str">
-        <f t="shared" ref="R45:S45" si="22">IF(NOT(M45=""),A45&amp;","&amp;M45,"")</f>
+      <c r="T45" s="6">
+        <f t="shared" si="3"/>
+        <v>0.92</v>
+      </c>
+      <c r="U45" s="12"/>
+      <c r="V45" s="4" t="str">
+        <f t="shared" ref="V45" si="21">IF(NOT(M45=""),A45&amp;","&amp;M45,"")</f>
         <v>1,ULN2803APGCN-ND</v>
       </c>
-      <c r="S45" s="4" t="str">
+      <c r="W45" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,ULN2803APGCN-ND</v>
       </c>
-      <c r="T45" t="str">
-        <f t="shared" ref="T45" si="23">A45&amp;"x "&amp;E45</f>
+      <c r="X45" t="str">
+        <f t="shared" ref="X45" si="22">A45&amp;"x "&amp;E45</f>
         <v>1x ULN2803APG</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y45" t="str">
+        <f t="shared" si="6"/>
+        <v>ULN2803A|1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <v>3</v>
       </c>
@@ -3893,13 +4712,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -3907,40 +4726,58 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N46" s="6">
+        <v>99</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O46" s="6">
         <v>0.5</v>
       </c>
-      <c r="O46" s="6">
-        <f>N46*A46</f>
+      <c r="P46" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="Q46" s="6">
+        <f>O46*A46</f>
         <v>1.5</v>
       </c>
-      <c r="P46" s="6">
+      <c r="R46" s="6">
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="S46" s="6">
+        <f>O46*B46</f>
+        <v>1</v>
+      </c>
+      <c r="T46" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4" t="str">
-        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4" t="str">
+        <f>IF(NOT(M46=""),A46&amp;","&amp;M46,"")</f>
         <v>3,AE10011-ND</v>
       </c>
-      <c r="S46" s="4" t="str">
+      <c r="W46" s="4" t="str">
         <f t="shared" si="4"/>
         <v>2,AE10011-ND</v>
       </c>
-      <c r="T46" t="str">
-        <f t="shared" si="9"/>
+      <c r="X46" t="str">
+        <f t="shared" si="10"/>
         <v>3x IC Socket</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y46" t="str">
+        <f t="shared" si="6"/>
+        <v>AR08-HZL-TT-R|3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="4"/>
@@ -3954,20 +4791,28 @@
       <c r="K47" s="4"/>
       <c r="L47" s="9"/>
       <c r="M47" s="3"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
       <c r="Q47" s="10"/>
-      <c r="R47" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="6"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="4" t="str">
+        <f>IF(NOT(M47=""),A47&amp;","&amp;M47,"")</f>
         <v/>
       </c>
-      <c r="S47" s="4" t="str">
+      <c r="W47" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y47" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>1</v>
       </c>
@@ -3975,10 +4820,10 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3988,37 +4833,55 @@
         <v>1</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="N48" s="6">
+        <v>201</v>
+      </c>
+      <c r="N48" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="O48" s="6">
         <v>15.33</v>
       </c>
-      <c r="O48" s="6">
-        <f>N48*A48</f>
+      <c r="P48" s="6">
         <v>15.33</v>
       </c>
-      <c r="P48" s="6">
+      <c r="Q48" s="6">
+        <f>O48*A48</f>
+        <v>15.33</v>
+      </c>
+      <c r="R48" s="6">
+        <f>P48*A48</f>
+        <v>15.33</v>
+      </c>
+      <c r="S48" s="6">
+        <f>O48*B48</f>
+        <v>15.33</v>
+      </c>
+      <c r="T48" s="6">
         <f t="shared" si="3"/>
         <v>15.33</v>
       </c>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="4" t="str">
+        <f>IF(NOT(M48=""),A48&amp;","&amp;M48,"")</f>
         <v>1,HM975-ND</v>
       </c>
-      <c r="S48" s="4" t="str">
+      <c r="W48" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1,HM975-ND</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y48" t="str">
+        <f t="shared" si="6"/>
+        <v>1455N1202|1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="4"/>
@@ -4032,27 +4895,31 @@
       <c r="K49" s="4"/>
       <c r="L49" s="9"/>
       <c r="M49" s="3"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
       <c r="Q49" s="10"/>
-      <c r="R49" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="10"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="10"/>
+      <c r="V49" s="4" t="str">
+        <f>IF(NOT(M49=""),A49&amp;","&amp;M49,"")</f>
         <v/>
       </c>
-      <c r="S49" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="W49" s="4" t="str">
+        <f>IF(NOT(O49=""),B49&amp;","&amp;O49,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -4063,32 +4930,36 @@
       <c r="K50" s="8"/>
       <c r="L50" s="4"/>
       <c r="M50" s="3"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4" t="str">
+        <f>IF(NOT(M50=""),A50&amp;","&amp;M50,"")</f>
         <v/>
       </c>
-      <c r="S50" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="W50" s="4" t="str">
+        <f>IF(NOT(O50=""),B50&amp;","&amp;O50,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>1</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -4097,38 +4968,47 @@
         <v>1</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M51" s="3"/>
-      <c r="N51" s="6">
+      <c r="N51" s="3"/>
+      <c r="O51" s="6">
         <v>15</v>
       </c>
-      <c r="O51" s="6">
-        <f>N51*A51</f>
+      <c r="P51" s="6">
         <v>15</v>
       </c>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4" t="str">
+      <c r="Q51" s="6">
+        <f>O51*A51</f>
+        <v>15</v>
+      </c>
+      <c r="R51" s="6">
         <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="S51" s="6"/>
+      <c r="T51" s="6"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4" t="str">
+        <f>IF(NOT(M51=""),A51&amp;","&amp;M51,"")</f>
         <v/>
       </c>
-      <c r="S51" s="4"/>
-    </row>
-    <row r="52" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W51" s="4"/>
+    </row>
+    <row r="52" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>1</v>
       </c>
       <c r="B52" s="17"/>
       <c r="C52" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -4139,18 +5019,22 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="N52" s="3">
+        <v>111</v>
+      </c>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3">
         <v>61.65</v>
       </c>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-      <c r="Q52" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P52" s="3"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+      <c r="U52" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="4"/>
@@ -4162,23 +5046,33 @@
       <c r="I53" s="8"/>
       <c r="J53" s="4"/>
       <c r="K53" s="8"/>
-      <c r="L53" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="M53" s="28"/>
-      <c r="N53" s="1" t="s">
+      <c r="L53" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="M53" s="29"/>
+      <c r="N53" s="27"/>
+      <c r="O53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="11">
+        <f>SUM(Q2:Q52)</f>
+        <v>103.13200000000001</v>
+      </c>
+      <c r="R53" s="11">
+        <f>SUM(R2:R52)</f>
+        <v>105.52000000000001</v>
+      </c>
+      <c r="S53" s="11">
+        <f>SUM(S2:S52)</f>
+        <v>76.871999999999986</v>
+      </c>
+      <c r="T53" s="11">
+        <f>SUM(T2:T52)</f>
+        <v>81.3</v>
+      </c>
+      <c r="U53" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="O53" s="11">
-        <f>SUM(O2:O52)</f>
-        <v>103.13200000000001</v>
-      </c>
-      <c r="P53" s="11">
-        <f>SUM(P2:P52)</f>
-        <v>76.871999999999986</v>
-      </c>
-      <c r="Q53" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed 2 unneeded resistors
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/v0.4_bom.xlsx
+++ b/reference/hardware/v0.4/v0.4_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -456,9 +456,6 @@
     <t>LED current limiting resistors</t>
   </si>
   <si>
-    <t>R39, 40,54,59,60</t>
-  </si>
-  <si>
     <t>S1012EC-40-ND</t>
   </si>
   <si>
@@ -877,6 +874,9 @@
   </si>
   <si>
     <t>863-1N5919BRLG</t>
+  </si>
+  <si>
+    <t>R39, 40,54</t>
   </si>
 </sst>
 </file>
@@ -1193,18 +1193,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1600,8 +1600,8 @@
   </sheetPr>
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J20" workbookViewId="0">
-      <selection activeCell="U36" sqref="U36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1621,16 +1621,16 @@
   <sheetData>
     <row r="1" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1651,7 +1651,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1660,40 +1660,40 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="V1" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="W1" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="X1" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y1" s="21" t="s">
         <v>219</v>
-      </c>
-      <c r="X1" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y1" s="21" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4" t="str">
-        <f>IF(NOT(M2=""),A2&amp;","&amp;M2,"")</f>
+        <f t="shared" ref="V2:V24" si="0">IF(NOT(M2=""),A2&amp;","&amp;M2,"")</f>
         <v/>
       </c>
       <c r="W2" s="4" t="str">
@@ -1737,7 +1737,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="20">
-        <f t="shared" ref="B3:B10" si="0">LEN(D3)-LEN(SUBSTITUTE(D3,",",""))+1</f>
+        <f t="shared" ref="B3:B10" si="1">LEN(D3)-LEN(SUBSTITUTE(D3,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1750,7 +1750,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -1763,16 +1763,16 @@
         <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O3" s="5">
         <v>1.7</v>
@@ -1781,7 +1781,7 @@
         <v>1.7</v>
       </c>
       <c r="Q3" s="6">
-        <f t="shared" ref="Q3:Q10" si="1">O3*A3</f>
+        <f t="shared" ref="Q3:Q10" si="2">O3*A3</f>
         <v>1.7</v>
       </c>
       <c r="R3" s="6">
@@ -1789,7 +1789,7 @@
         <v>1.7</v>
       </c>
       <c r="S3" s="6">
-        <f>O3*B3</f>
+        <f t="shared" ref="S3:S10" si="3">O3*B3</f>
         <v>1.7</v>
       </c>
       <c r="T3" s="6">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="U3" s="4"/>
       <c r="V3" s="4" t="str">
-        <f>IF(NOT(M3=""),A3&amp;","&amp;M3,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-3654-ND</v>
       </c>
       <c r="W3" s="4" t="str">
@@ -1820,7 +1820,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1833,7 +1833,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -1846,16 +1846,16 @@
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O4" s="5">
         <v>0.66</v>
@@ -1864,36 +1864,36 @@
         <v>0.66</v>
       </c>
       <c r="Q4" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="R4" s="6">
-        <f t="shared" ref="R4:R51" si="2">P4*A4</f>
+        <f t="shared" ref="R4:R51" si="4">P4*A4</f>
         <v>3.3000000000000003</v>
       </c>
       <c r="S4" s="6">
-        <f>O4*B4</f>
+        <f t="shared" si="3"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="T4" s="6">
-        <f t="shared" ref="T4:T48" si="3">P4*B4</f>
+        <f t="shared" ref="T4:T48" si="5">P4*B4</f>
         <v>3.3000000000000003</v>
       </c>
       <c r="U4" s="4"/>
       <c r="V4" s="4" t="str">
-        <f>IF(NOT(M4=""),A4&amp;","&amp;M4,"")</f>
+        <f t="shared" si="0"/>
         <v>5,399-4353-ND</v>
       </c>
       <c r="W4" s="4" t="str">
-        <f t="shared" ref="W4:W48" si="4">IF(NOT(M4=""),B4&amp;","&amp;M4,"")</f>
+        <f t="shared" ref="W4:W48" si="6">IF(NOT(M4=""),B4&amp;","&amp;M4,"")</f>
         <v>5,399-4353-ND</v>
       </c>
       <c r="X4" t="str">
-        <f t="shared" ref="X4:X10" si="5">"Capacitor - " &amp;A4&amp;"x "&amp;E4</f>
+        <f t="shared" ref="X4:X10" si="7">"Capacitor - " &amp;A4&amp;"x "&amp;E4</f>
         <v>Capacitor - 5x 0.22uF</v>
       </c>
       <c r="Y4" t="str">
-        <f t="shared" ref="Y4:Y48" si="6">IF(NOT(N4=""),N4&amp;"|"&amp;A4,"")</f>
+        <f t="shared" ref="Y4:Y48" si="8">IF(NOT(N4=""),N4&amp;"|"&amp;A4,"")</f>
         <v>80-C322C224K5R|5</v>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1916,7 +1916,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -1929,16 +1929,16 @@
         <v>13</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="N5" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O5" s="5">
         <v>0.32</v>
@@ -1947,36 +1947,36 @@
         <v>0.32</v>
       </c>
       <c r="Q5" s="6">
-        <f t="shared" si="1"/>
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="R5" s="6">
         <f t="shared" si="2"/>
         <v>2.2400000000000002</v>
       </c>
+      <c r="R5" s="6">
+        <f t="shared" si="4"/>
+        <v>2.2400000000000002</v>
+      </c>
       <c r="S5" s="6">
-        <f>O5*B5</f>
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="T5" s="6">
         <f t="shared" si="3"/>
         <v>2.2400000000000002</v>
       </c>
+      <c r="T5" s="6">
+        <f t="shared" si="5"/>
+        <v>2.2400000000000002</v>
+      </c>
       <c r="U5" s="4"/>
       <c r="V5" s="4" t="str">
-        <f>IF(NOT(M5=""),A5&amp;","&amp;M5,"")</f>
+        <f t="shared" si="0"/>
         <v>7,399-9879-1-ND</v>
       </c>
       <c r="W5" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7,399-9879-1-ND</v>
       </c>
       <c r="X5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>80-C322C104M5R-TR|7</v>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1999,7 +1999,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>9</v>
@@ -2012,16 +2012,16 @@
         <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="N6" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O6" s="5">
         <v>1.57</v>
@@ -2030,46 +2030,46 @@
         <v>1.57</v>
       </c>
       <c r="Q6" s="6">
-        <f t="shared" si="1"/>
-        <v>1.57</v>
-      </c>
-      <c r="R6" s="6">
         <f t="shared" si="2"/>
         <v>1.57</v>
       </c>
+      <c r="R6" s="6">
+        <f t="shared" si="4"/>
+        <v>1.57</v>
+      </c>
       <c r="S6" s="6">
-        <f>O6*B6</f>
-        <v>1.57</v>
-      </c>
-      <c r="T6" s="6">
         <f t="shared" si="3"/>
         <v>1.57</v>
       </c>
+      <c r="T6" s="6">
+        <f t="shared" si="5"/>
+        <v>1.57</v>
+      </c>
       <c r="U6" s="4"/>
       <c r="V6" s="4" t="str">
-        <f>IF(NOT(M6=""),A6&amp;","&amp;M6,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-3652-ND</v>
       </c>
       <c r="W6" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,399-3652-ND</v>
       </c>
       <c r="X6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Capacitor - 1x 47uF</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>80-T356F476K6AT|1</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
-        <f t="shared" ref="A7:A9" si="7">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
+        <f t="shared" ref="A7:A9" si="9">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B7" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2082,7 +2082,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -2095,16 +2095,16 @@
         <v>10</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="N7" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O7" s="5">
         <v>0.62</v>
@@ -2113,46 +2113,46 @@
         <v>0.43</v>
       </c>
       <c r="Q7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.62</v>
       </c>
       <c r="R7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.43</v>
       </c>
       <c r="S7" s="6">
-        <f>O7*B7</f>
+        <f t="shared" si="3"/>
         <v>0.62</v>
       </c>
       <c r="T7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.43</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4" t="str">
-        <f>IF(NOT(M7=""),A7&amp;","&amp;M7,"")</f>
+        <f t="shared" si="0"/>
         <v>1,478-5120-ND</v>
       </c>
       <c r="W7" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,478-5120-ND</v>
       </c>
       <c r="X7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Capacitor - 1x 0.33uF</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>581-AR215F334K4R|1</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B8" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -2165,7 +2165,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -2178,16 +2178,16 @@
         <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="N8" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O8" s="5">
         <v>0.24</v>
@@ -2196,59 +2196,59 @@
         <v>0.24</v>
       </c>
       <c r="Q8" s="6">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="R8" s="6">
         <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
+      <c r="R8" s="6">
+        <f t="shared" si="4"/>
+        <v>0.24</v>
+      </c>
       <c r="S8" s="6">
-        <f>O8*B8</f>
-        <v>0.24</v>
-      </c>
-      <c r="T8" s="6">
         <f t="shared" si="3"/>
         <v>0.24</v>
       </c>
+      <c r="T8" s="6">
+        <f t="shared" si="5"/>
+        <v>0.24</v>
+      </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4" t="str">
-        <f>IF(NOT(M8=""),A8&amp;","&amp;M8,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-4206-ND</v>
       </c>
       <c r="W8" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,399-4206-ND</v>
       </c>
       <c r="X8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Capacitor - 1x 0.01uF</v>
       </c>
       <c r="Y8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>80-C317C103K5R|1</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B9" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>12</v>
@@ -2261,16 +2261,16 @@
         <v>13</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="N9" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O9" s="5">
         <v>0.66</v>
@@ -2279,36 +2279,36 @@
         <v>0.66</v>
       </c>
       <c r="Q9" s="6">
-        <f t="shared" si="1"/>
-        <v>1.98</v>
-      </c>
-      <c r="R9" s="6">
         <f t="shared" si="2"/>
         <v>1.98</v>
       </c>
+      <c r="R9" s="6">
+        <f t="shared" si="4"/>
+        <v>1.98</v>
+      </c>
       <c r="S9" s="6">
-        <f>O9*B9</f>
-        <v>1.32</v>
-      </c>
-      <c r="T9" s="6">
         <f t="shared" si="3"/>
         <v>1.32</v>
       </c>
+      <c r="T9" s="6">
+        <f t="shared" si="5"/>
+        <v>1.32</v>
+      </c>
       <c r="U9" s="4"/>
       <c r="V9" s="4" t="str">
-        <f>IF(NOT(M9=""),A9&amp;","&amp;M9,"")</f>
+        <f t="shared" si="0"/>
         <v>3,399-4390-ND</v>
       </c>
       <c r="W9" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2,399-4390-ND</v>
       </c>
       <c r="X9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Capacitor - 3x 1uF</v>
       </c>
       <c r="Y9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>80-C330C105M5U|3</v>
       </c>
     </row>
@@ -2318,20 +2318,20 @@
         <v>1</v>
       </c>
       <c r="B10" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
@@ -2342,16 +2342,16 @@
         <v>13</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O10" s="5">
         <v>0.25</v>
@@ -2360,36 +2360,36 @@
         <v>0.25</v>
       </c>
       <c r="Q10" s="6">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="R10" s="6">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
+      <c r="R10" s="6">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
       <c r="S10" s="6">
-        <f>O10*B10</f>
-        <v>0.25</v>
-      </c>
-      <c r="T10" s="6">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
+      <c r="T10" s="6">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
       <c r="U10" s="4"/>
       <c r="V10" s="4" t="str">
-        <f>IF(NOT(M10=""),A10&amp;","&amp;M10,"")</f>
+        <f t="shared" si="0"/>
         <v>1,399-4243-ND</v>
       </c>
       <c r="W10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,399-4243-ND</v>
       </c>
       <c r="X10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Capacitor - 1x 4.7nF</v>
       </c>
       <c r="Y10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>80-C317C472K1R|1</v>
       </c>
     </row>
@@ -2416,15 +2416,15 @@
       <c r="T11" s="6"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4" t="str">
-        <f>IF(NOT(M11=""),A11&amp;","&amp;M11,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="W11" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -2451,15 +2451,15 @@
       <c r="T12" s="6"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4" t="str">
-        <f>IF(NOT(M12=""),A12&amp;","&amp;M12,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="W12" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="20">
-        <f t="shared" ref="B13:B16" si="8">LEN(D13)-LEN(SUBSTITUTE(D13,",",""))+1</f>
+        <f t="shared" ref="B13:B16" si="10">LEN(D13)-LEN(SUBSTITUTE(D13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2479,7 +2479,7 @@
         <v>92</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>19</v>
@@ -2495,7 +2495,7 @@
         <v>21</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>22</v>
@@ -2504,7 +2504,7 @@
         <v>23</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O13" s="5">
         <v>0.34</v>
@@ -2517,7 +2517,7 @@
         <v>0.34</v>
       </c>
       <c r="R13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.43</v>
       </c>
       <c r="S13" s="6">
@@ -2525,16 +2525,16 @@
         <v>0.34</v>
       </c>
       <c r="T13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.43</v>
       </c>
       <c r="U13" s="4"/>
       <c r="V13" s="4" t="str">
-        <f>IF(NOT(M13=""),A13&amp;","&amp;M13,"")</f>
+        <f t="shared" si="0"/>
         <v>1,1N5919BGOS-ND</v>
       </c>
       <c r="W13" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,1N5919BGOS-ND</v>
       </c>
       <c r="X13" t="str">
@@ -2542,7 +2542,7 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
       <c r="Y13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>863-1N5919BRLG|1</v>
       </c>
     </row>
@@ -2552,17 +2552,17 @@
         <v>12</v>
       </c>
       <c r="B14" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>25</v>
@@ -2578,7 +2578,7 @@
         <v>26</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>24</v>
@@ -2587,7 +2587,7 @@
         <v>27</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O14" s="5">
         <v>0.39</v>
@@ -2600,7 +2600,7 @@
         <v>4.68</v>
       </c>
       <c r="R14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.68</v>
       </c>
       <c r="S14" s="6">
@@ -2608,24 +2608,24 @@
         <v>4.68</v>
       </c>
       <c r="T14" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.68</v>
       </c>
       <c r="U14" s="4"/>
       <c r="V14" s="4" t="str">
-        <f>IF(NOT(M14=""),A14&amp;","&amp;M14,"")</f>
+        <f t="shared" si="0"/>
         <v>12,1N5818-TPCT-ND</v>
       </c>
       <c r="W14" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12,1N5818-TPCT-ND</v>
       </c>
       <c r="X14" t="str">
-        <f t="shared" ref="X14:X16" si="9">"Diode - " &amp;A14&amp;"x "&amp;E14</f>
+        <f t="shared" ref="X14:X16" si="11">"Diode - " &amp;A14&amp;"x "&amp;E14</f>
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
       <c r="Y14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>833-1N5818-TP|12</v>
       </c>
     </row>
@@ -2635,14 +2635,14 @@
         <v>8</v>
       </c>
       <c r="B15" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>28</v>
@@ -2657,14 +2657,14 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="2" t="s">
         <v>119</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O15" s="5">
         <v>0.47</v>
@@ -2677,7 +2677,7 @@
         <v>3.76</v>
       </c>
       <c r="R15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="S15" s="6">
@@ -2685,24 +2685,24 @@
         <v>1.88</v>
       </c>
       <c r="T15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
       <c r="U15" s="4"/>
       <c r="V15" s="4" t="str">
-        <f>IF(NOT(M15=""),A15&amp;","&amp;M15,"")</f>
+        <f t="shared" si="0"/>
         <v>8,160-1139-ND</v>
       </c>
       <c r="W15" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4,160-1139-ND</v>
       </c>
       <c r="X15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Diode - 8x LED-Red</v>
       </c>
       <c r="Y15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>859-LTL-4221N|8</v>
       </c>
     </row>
@@ -2712,14 +2712,14 @@
         <v>4</v>
       </c>
       <c r="B16" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>29</v>
@@ -2738,7 +2738,7 @@
         <v>26</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>31</v>
@@ -2747,7 +2747,7 @@
         <v>32</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O16" s="5">
         <v>0.11</v>
@@ -2760,7 +2760,7 @@
         <v>0.44</v>
       </c>
       <c r="R16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.44</v>
       </c>
       <c r="S16" s="6">
@@ -2768,24 +2768,24 @@
         <v>0.22</v>
       </c>
       <c r="T16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.22</v>
       </c>
       <c r="U16" s="4"/>
       <c r="V16" s="4" t="str">
-        <f>IF(NOT(M16=""),A16&amp;","&amp;M16,"")</f>
+        <f t="shared" si="0"/>
         <v>4,1N4004-TPMSCT-ND</v>
       </c>
       <c r="W16" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2,1N4004-TPMSCT-ND</v>
       </c>
       <c r="X16" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>Diode - 4x 1N4004</v>
       </c>
       <c r="Y16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>833-1N4004-TP|4</v>
       </c>
     </row>
@@ -2812,19 +2812,19 @@
       <c r="T17" s="6"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4" t="str">
-        <f>IF(NOT(M17=""),A17&amp;","&amp;M17,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="W17" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X17" t="str">
-        <f t="shared" ref="X17:X46" si="10">A17&amp;"x "&amp;E17</f>
+        <f t="shared" ref="X17:X46" si="12">A17&amp;"x "&amp;E17</f>
         <v xml:space="preserve">x </v>
       </c>
       <c r="Y17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -2851,19 +2851,19 @@
       <c r="T18" s="6"/>
       <c r="U18" s="3"/>
       <c r="V18" s="4" t="str">
-        <f>IF(NOT(M18=""),A18&amp;","&amp;M18,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="W18" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X18" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="Y18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -2890,19 +2890,19 @@
       <c r="T19" s="6"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4" t="str">
-        <f>IF(NOT(M19=""),A19&amp;","&amp;M19,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="W19" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X19" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="Y19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="20">
-        <f t="shared" ref="B20" si="11">LEN(D20)-LEN(SUBSTITUTE(D20,",",""))+1</f>
+        <f t="shared" ref="B20" si="13">LEN(D20)-LEN(SUBSTITUTE(D20,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2937,7 +2937,7 @@
         <v>36</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>37</v>
@@ -2946,7 +2946,7 @@
         <v>38</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O20" s="5">
         <v>0.72</v>
@@ -2959,32 +2959,32 @@
         <v>0.72</v>
       </c>
       <c r="R20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.72</v>
       </c>
       <c r="S20" s="6">
-        <f>O20*B20</f>
+        <f t="shared" ref="S20:S25" si="14">O20*B20</f>
         <v>0.72</v>
       </c>
       <c r="T20" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.72</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4" t="str">
-        <f>IF(NOT(M20=""),A20&amp;","&amp;M20,"")</f>
+        <f t="shared" si="0"/>
         <v>1,P7307-ND</v>
       </c>
       <c r="W20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,P7307-ND</v>
       </c>
       <c r="X20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1x Surge Protection</v>
       </c>
       <c r="Y20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>667-ERZ-V14D220|1</v>
       </c>
     </row>
@@ -3008,28 +3008,28 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6">
-        <f>O21*B21</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="T21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U21" s="4"/>
       <c r="V21" s="4" t="str">
-        <f>IF(NOT(M21=""),A21&amp;","&amp;M21,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="W21" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="Y21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3038,38 +3038,38 @@
         <v>1</v>
       </c>
       <c r="B22" s="20">
-        <f t="shared" ref="B22" si="12">LEN(D22)-LEN(SUBSTITUTE(D22,",",""))+1</f>
+        <f t="shared" ref="B22" si="15">LEN(D22)-LEN(SUBSTITUTE(D22,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O22" s="3">
         <v>0.40200000000000002</v>
@@ -3082,26 +3082,26 @@
         <v>0.40200000000000002</v>
       </c>
       <c r="R22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.51</v>
       </c>
       <c r="S22" s="6">
-        <f>O22*B22</f>
+        <f t="shared" si="14"/>
         <v>0.40200000000000002</v>
       </c>
       <c r="T22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.51</v>
       </c>
       <c r="U22" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V22" s="4" t="str">
-        <f>IF(NOT(M22=""),A22&amp;","&amp;M22,"")</f>
+        <f t="shared" si="0"/>
         <v>1,ED2561-ND</v>
       </c>
       <c r="W22" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,ED2561-ND</v>
       </c>
       <c r="X22" t="str">
@@ -3109,7 +3109,7 @@
         <v>1x Dual Terminal Block</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>571-2828362|1</v>
       </c>
     </row>
@@ -3121,10 +3121,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>39</v>
@@ -3137,16 +3137,16 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>109</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O23" s="5">
         <v>0.1</v>
@@ -3159,32 +3159,32 @@
         <v>0.5</v>
       </c>
       <c r="R23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="S23" s="6">
-        <f>O23*B23</f>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="T23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="4" t="str">
-        <f>IF(NOT(M23=""),A23&amp;","&amp;M23,"")</f>
+        <f t="shared" si="0"/>
         <v>5,3M9580-ND</v>
       </c>
       <c r="W23" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5,3M9580-ND</v>
       </c>
       <c r="X23" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5x Jumper</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>517-9691020000DA|5</v>
       </c>
     </row>
@@ -3202,10 +3202,10 @@
         <v>114</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -3213,24 +3213,24 @@
         <v>1</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="N24" s="31" t="s">
-        <v>260</v>
+        <v>124</v>
+      </c>
+      <c r="N24" s="29" t="s">
+        <v>259</v>
       </c>
       <c r="O24" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="P24" s="32">
+      <c r="P24" s="30">
         <v>2.95</v>
       </c>
       <c r="Q24" s="6">
@@ -3238,38 +3238,38 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="R24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.9</v>
       </c>
       <c r="S24" s="6">
-        <f>O24*B24</f>
+        <f t="shared" si="14"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="T24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.9</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="V24" s="4" t="str">
-        <f>IF(NOT(M24=""),A24&amp;","&amp;M24,"")</f>
+        <f t="shared" si="0"/>
         <v>2,S1012EC-40-ND</v>
       </c>
       <c r="W24" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2,S1012EC-40-ND</v>
       </c>
       <c r="X24" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2x 40 POS 0.100 Pin Header</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>782-A000026|2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="53" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>1</v>
       </c>
@@ -3277,16 +3277,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3294,19 +3294,19 @@
         <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="M25" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O25" s="6">
         <v>1.1299999999999999</v>
@@ -3319,32 +3319,32 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="R25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="S25" s="6">
-        <f>O25*B25</f>
+        <f t="shared" si="14"/>
         <v>1.1299999999999999</v>
       </c>
       <c r="T25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4" t="str">
-        <f t="shared" ref="V25" si="13">IF(NOT(M25=""),A25&amp;","&amp;M25,"")</f>
+        <f t="shared" ref="V25" si="16">IF(NOT(M25=""),A25&amp;","&amp;M25,"")</f>
         <v>1,1175-1614-ND</v>
       </c>
       <c r="W25" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,1175-1614-ND</v>
       </c>
       <c r="X25" t="str">
-        <f t="shared" ref="X25" si="14">A25&amp;"x "&amp;E25</f>
+        <f t="shared" ref="X25" si="17">A25&amp;"x "&amp;E25</f>
         <v>1x Rectangular Connectors - Headers, Male Pins</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>571-5103308-8|1</v>
       </c>
     </row>
@@ -3371,19 +3371,19 @@
       <c r="T26" s="6"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4" t="str">
-        <f>IF(NOT(M26=""),A26&amp;","&amp;M26,"")</f>
+        <f t="shared" ref="V26:V44" si="18">IF(NOT(M26=""),A26&amp;","&amp;M26,"")</f>
         <v/>
       </c>
       <c r="W26" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3410,19 +3410,19 @@
       <c r="T27" s="6"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4" t="str">
-        <f>IF(NOT(M27=""),A27&amp;","&amp;M27,"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="W27" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X27" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">x </v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3432,17 +3432,17 @@
         <v>8</v>
       </c>
       <c r="B28" s="20">
-        <f t="shared" ref="B28" si="15">LEN(D28)-LEN(SUBSTITUTE(D28,",",""))+1</f>
+        <f t="shared" ref="B28" si="19">LEN(D28)-LEN(SUBSTITUTE(D28,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>116</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>107</v>
@@ -3458,7 +3458,7 @@
         <v>40</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>108</v>
@@ -3467,7 +3467,7 @@
         <v>106</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O28" s="6">
         <v>1.51</v>
@@ -3480,7 +3480,7 @@
         <v>12.08</v>
       </c>
       <c r="R28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12.08</v>
       </c>
       <c r="S28" s="6">
@@ -3488,12 +3488,12 @@
         <v>9.06</v>
       </c>
       <c r="T28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.06</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="4" t="str">
-        <f>IF(NOT(M28=""),A28&amp;","&amp;M28,"")</f>
+        <f t="shared" si="18"/>
         <v>8,497-5896-5-ND</v>
       </c>
       <c r="W28" s="4" t="str">
@@ -3501,11 +3501,11 @@
         <v>6,497-5896-5-ND</v>
       </c>
       <c r="X28" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8x 62A MOSFET N-CH</v>
       </c>
       <c r="Y28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>511-STP62NS04Z|8</v>
       </c>
     </row>
@@ -3532,15 +3532,15 @@
       <c r="T29" s="6"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4" t="str">
-        <f>IF(NOT(M29=""),A29&amp;","&amp;M29,"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="W29" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -3567,32 +3567,32 @@
       <c r="T30" s="6"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4" t="str">
-        <f>IF(NOT(M30=""),A30&amp;","&amp;M30,"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="W30" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <f>LEN(C31)-LEN(SUBSTITUTE(C31,",",""))+1</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31" s="20">
-        <f t="shared" ref="B31:B37" si="16">LEN(D31)-LEN(SUBSTITUTE(D31,",",""))+1</f>
-        <v>5</v>
+        <f t="shared" ref="B31:B37" si="20">LEN(D31)-LEN(SUBSTITUTE(D31,",",""))+1</f>
+        <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>124</v>
+        <v>264</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>124</v>
+        <v>264</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>41</v>
@@ -3609,7 +3609,7 @@
         <v>43</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>44</v>
@@ -3618,7 +3618,7 @@
         <v>45</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O31" s="5">
         <v>0.08</v>
@@ -3627,37 +3627,37 @@
         <v>0.11</v>
       </c>
       <c r="Q31" s="6">
-        <f t="shared" ref="Q31:Q39" si="17">O31*A31</f>
-        <v>0.4</v>
+        <f t="shared" ref="Q31:Q39" si="21">O31*A31</f>
+        <v>0.24</v>
       </c>
       <c r="R31" s="6">
-        <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <f t="shared" si="4"/>
+        <v>0.33</v>
       </c>
       <c r="S31" s="6">
-        <f>O31*B31</f>
-        <v>0.4</v>
+        <f t="shared" ref="S31:S39" si="22">O31*B31</f>
+        <v>0.24</v>
       </c>
       <c r="T31" s="6">
-        <f t="shared" si="3"/>
-        <v>0.55000000000000004</v>
+        <f t="shared" si="5"/>
+        <v>0.33</v>
       </c>
       <c r="U31" s="4"/>
       <c r="V31" s="4" t="str">
-        <f>IF(NOT(M31=""),A31&amp;","&amp;M31,"")</f>
-        <v>5,10.0KXBK-ND</v>
+        <f t="shared" si="18"/>
+        <v>3,10.0KXBK-ND</v>
       </c>
       <c r="W31" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>5,10.0KXBK-ND</v>
+        <f t="shared" si="6"/>
+        <v>3,10.0KXBK-ND</v>
       </c>
       <c r="X31" t="str">
         <f>"Resistor - " &amp; A31&amp;"x "&amp;E31</f>
-        <v>Resistor - 5x 10k</v>
+        <v>Resistor - 3x 10k</v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="6"/>
-        <v>71-RN60D-F-10K|5</v>
+        <f t="shared" si="8"/>
+        <v>71-RN60D-F-10K|3</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3666,14 +3666,14 @@
         <v>12</v>
       </c>
       <c r="B32" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>46</v>
@@ -3690,7 +3690,7 @@
         <v>43</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>48</v>
@@ -3699,7 +3699,7 @@
         <v>49</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O32" s="5">
         <v>0.06</v>
@@ -3708,36 +3708,36 @@
         <v>0.11</v>
       </c>
       <c r="Q32" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.72</v>
       </c>
       <c r="R32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.32</v>
       </c>
       <c r="S32" s="6">
-        <f>O32*B32</f>
+        <f t="shared" si="22"/>
         <v>0.48</v>
       </c>
       <c r="T32" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.88</v>
       </c>
       <c r="U32" s="4"/>
       <c r="V32" s="4" t="str">
-        <f>IF(NOT(M32=""),A32&amp;","&amp;M32,"")</f>
+        <f t="shared" si="18"/>
         <v>12,1.00KXBK-ND</v>
       </c>
       <c r="W32" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8,1.00KXBK-ND</v>
       </c>
       <c r="X32" t="str">
-        <f t="shared" ref="X32:X39" si="18">"Resistor - " &amp; A32&amp;"x "&amp;E32</f>
+        <f t="shared" ref="X32:X39" si="23">"Resistor - " &amp; A32&amp;"x "&amp;E32</f>
         <v>Resistor - 12x 1k</v>
       </c>
       <c r="Y32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>71-RN60D-F-1.0K|12</v>
       </c>
     </row>
@@ -3747,36 +3747,36 @@
         <v>8</v>
       </c>
       <c r="B33" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>115</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E33" s="13">
         <v>680</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L33" s="7"/>
       <c r="M33" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O33" s="14">
         <v>0.22</v>
@@ -3785,38 +3785,38 @@
         <v>0.15</v>
       </c>
       <c r="Q33" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.76</v>
       </c>
       <c r="R33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
       <c r="S33" s="6">
-        <f>O33*B33</f>
+        <f t="shared" si="22"/>
         <v>0.88</v>
       </c>
       <c r="T33" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="U33" s="12" t="s">
         <v>123</v>
       </c>
       <c r="V33" s="4" t="str">
-        <f>IF(NOT(M33=""),A33&amp;","&amp;M33,"")</f>
+        <f t="shared" si="18"/>
         <v>8,A105963CT-ND</v>
       </c>
       <c r="W33" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4,A105963CT-ND</v>
       </c>
       <c r="X33" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>Resistor - 8x 680</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>279-LR1F680R|8</v>
       </c>
     </row>
@@ -3826,14 +3826,14 @@
         <v>6</v>
       </c>
       <c r="B34" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E34" s="3">
         <v>470</v>
@@ -3850,7 +3850,7 @@
         <v>51</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>52</v>
@@ -3859,7 +3859,7 @@
         <v>53</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O34" s="5">
         <v>0.11</v>
@@ -3868,36 +3868,36 @@
         <v>0.15</v>
       </c>
       <c r="Q34" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.66</v>
       </c>
       <c r="R34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="S34" s="6">
-        <f>O34*B34</f>
+        <f t="shared" si="22"/>
         <v>0.66</v>
       </c>
       <c r="T34" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="U34" s="4"/>
       <c r="V34" s="4" t="str">
-        <f>IF(NOT(M34=""),A34&amp;","&amp;M34,"")</f>
+        <f t="shared" si="18"/>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
       <c r="W34" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
       <c r="X34" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>Resistor - 6x 470</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>279-LR1F470R|6</v>
       </c>
     </row>
@@ -3906,7 +3906,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -3916,7 +3916,7 @@
         <v>85</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>54</v>
@@ -3932,7 +3932,7 @@
         <v>56</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>57</v>
@@ -3941,7 +3941,7 @@
         <v>58</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O35" s="5">
         <v>1.92</v>
@@ -3950,36 +3950,36 @@
         <v>1.92</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>3.84</v>
       </c>
       <c r="R35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.84</v>
       </c>
       <c r="S35" s="6">
-        <f>O35*B35</f>
+        <f t="shared" si="22"/>
         <v>3.84</v>
       </c>
       <c r="T35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.84</v>
       </c>
       <c r="U35" s="4"/>
       <c r="V35" s="4" t="str">
-        <f>IF(NOT(M35=""),A35&amp;","&amp;M35,"")</f>
+        <f t="shared" si="18"/>
         <v>2,985-1047-1-ND</v>
       </c>
       <c r="W35" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2,985-1047-1-ND</v>
       </c>
       <c r="X35" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>756-RC55Y-2K49BI|2</v>
       </c>
     </row>
@@ -3988,7 +3988,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -3998,7 +3998,7 @@
         <v>86</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>59</v>
@@ -4012,7 +4012,7 @@
         <v>43</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>60</v>
@@ -4021,7 +4021,7 @@
         <v>61</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O36" s="5">
         <v>0.46</v>
@@ -4030,38 +4030,38 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="Q36" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.46</v>
       </c>
       <c r="R36" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="S36" s="6">
-        <f>O36*B36</f>
+        <f t="shared" si="22"/>
         <v>0.46</v>
       </c>
       <c r="T36" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="U36" s="4" t="s">
         <v>121</v>
       </c>
       <c r="V36" s="4" t="str">
-        <f>IF(NOT(M36=""),A36&amp;","&amp;M36,"")</f>
+        <f t="shared" si="18"/>
         <v>1,3.9KADCT-ND</v>
       </c>
       <c r="W36" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,3.9KADCT-ND</v>
       </c>
       <c r="X36" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>279-H83K9BDA|1</v>
       </c>
     </row>
@@ -4070,7 +4070,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -4080,7 +4080,7 @@
         <v>87</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>62</v>
@@ -4094,7 +4094,7 @@
         <v>43</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>63</v>
@@ -4103,7 +4103,7 @@
         <v>64</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O37" s="5">
         <v>0.46</v>
@@ -4112,44 +4112,44 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="Q37" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.46</v>
       </c>
       <c r="R37" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="S37" s="6">
-        <f>O37*B37</f>
+        <f t="shared" si="22"/>
         <v>0.46</v>
       </c>
       <c r="T37" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="U37" s="4" t="s">
         <v>121</v>
       </c>
       <c r="V37" s="4" t="str">
-        <f>IF(NOT(M37=""),A37&amp;","&amp;M37,"")</f>
+        <f t="shared" si="18"/>
         <v>1,1KADCT-ND</v>
       </c>
       <c r="W37" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,1KADCT-ND</v>
       </c>
       <c r="X37" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>279-YR1B1K0CC|1</v>
       </c>
     </row>
     <row r="38" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
-        <f t="shared" ref="A38:A39" si="19">LEN(C38)-LEN(SUBSTITUTE(C38,",",""))+1</f>
+        <f t="shared" ref="A38:A39" si="24">LEN(C38)-LEN(SUBSTITUTE(C38,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B38" s="20">
@@ -4160,7 +4160,7 @@
         <v>122</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>65</v>
@@ -4177,7 +4177,7 @@
         <v>43</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>67</v>
@@ -4186,7 +4186,7 @@
         <v>68</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O38" s="5">
         <v>0.1</v>
@@ -4195,42 +4195,42 @@
         <v>0.1</v>
       </c>
       <c r="Q38" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="R38" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="S38" s="6">
-        <f>O38*B38</f>
+        <f t="shared" si="22"/>
         <v>0.8</v>
       </c>
       <c r="T38" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
       <c r="U38" s="4"/>
       <c r="V38" s="4" t="str">
-        <f>IF(NOT(M38=""),A38&amp;","&amp;M38,"")</f>
+        <f t="shared" si="18"/>
         <v>12,100KXBK-ND</v>
       </c>
       <c r="W38" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8,100KXBK-ND</v>
       </c>
       <c r="X38" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>Resistor - 12x 100k</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>603-MFR-25FBF52-100K|12</v>
       </c>
     </row>
     <row r="39" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="B39" s="20">
@@ -4241,7 +4241,7 @@
         <v>88</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E39" s="3">
         <v>160</v>
@@ -4258,7 +4258,7 @@
         <v>43</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>70</v>
@@ -4267,7 +4267,7 @@
         <v>71</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O39" s="5">
         <v>0.27</v>
@@ -4276,36 +4276,36 @@
         <v>0.23</v>
       </c>
       <c r="Q39" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.08</v>
       </c>
       <c r="R39" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.92</v>
       </c>
       <c r="S39" s="6">
-        <f>O39*B39</f>
+        <f t="shared" si="22"/>
         <v>0.54</v>
       </c>
       <c r="T39" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.46</v>
       </c>
       <c r="U39" s="4"/>
       <c r="V39" s="4" t="str">
-        <f>IF(NOT(M39=""),A39&amp;","&amp;M39,"")</f>
+        <f t="shared" si="18"/>
         <v>4,160YCT-ND</v>
       </c>
       <c r="W39" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2,160YCT-ND</v>
       </c>
       <c r="X39" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>Resistor - 4x 160</v>
       </c>
       <c r="Y39" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>594-5083NW160R0J|4</v>
       </c>
     </row>
@@ -4332,15 +4332,15 @@
       <c r="T40" s="6"/>
       <c r="U40" s="4"/>
       <c r="V40" s="4" t="str">
-        <f>IF(NOT(M40=""),A40&amp;","&amp;M40,"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="W40" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -4367,15 +4367,15 @@
       <c r="T41" s="6"/>
       <c r="U41" s="4"/>
       <c r="V41" s="4" t="str">
-        <f>IF(NOT(M41=""),A41&amp;","&amp;M41,"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="W41" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -4384,7 +4384,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="20">
-        <f t="shared" ref="B42:B44" si="20">LEN(D42)-LEN(SUBSTITUTE(D42,",",""))+1</f>
+        <f t="shared" ref="B42:B44" si="25">LEN(D42)-LEN(SUBSTITUTE(D42,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -4410,7 +4410,7 @@
         <v>77</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>74</v>
@@ -4419,7 +4419,7 @@
         <v>74</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O42" s="5">
         <v>1.68</v>
@@ -4432,7 +4432,7 @@
         <v>1.68</v>
       </c>
       <c r="R42" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.67</v>
       </c>
       <c r="S42" s="6">
@@ -4440,24 +4440,24 @@
         <v>1.68</v>
       </c>
       <c r="T42" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.67</v>
       </c>
       <c r="U42" s="4"/>
       <c r="V42" s="4" t="str">
-        <f>IF(NOT(M42=""),A42&amp;","&amp;M42,"")</f>
+        <f t="shared" si="18"/>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
       <c r="W42" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
       <c r="X42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>926-LM2940T-5.0/NOPB|1</v>
       </c>
     </row>
@@ -4466,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -4476,7 +4476,7 @@
         <v>98</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>97</v>
@@ -4493,13 +4493,13 @@
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>95</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O43" s="6">
         <v>15.41</v>
@@ -4512,7 +4512,7 @@
         <v>15.41</v>
       </c>
       <c r="R43" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15.37</v>
       </c>
       <c r="S43" s="6">
@@ -4520,24 +4520,24 @@
         <v>15.41</v>
       </c>
       <c r="T43" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.37</v>
       </c>
       <c r="U43" s="4"/>
       <c r="V43" s="4" t="str">
-        <f>IF(NOT(M43=""),A43&amp;","&amp;M43,"")</f>
+        <f t="shared" si="18"/>
         <v>1,MPX4250AP-ND</v>
       </c>
       <c r="W43" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,MPX4250AP-ND</v>
       </c>
       <c r="X43" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1x 1-Bar MAP sensor</v>
       </c>
       <c r="Y43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>841-MPX4250AP|1</v>
       </c>
     </row>
@@ -4546,23 +4546,23 @@
         <v>2</v>
       </c>
       <c r="B44" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="C44" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E44" s="13" t="s">
+      <c r="F44" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="G44" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="13">
@@ -4572,16 +4572,16 @@
         <v>78</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O44" s="23">
         <v>2.92</v>
@@ -4594,7 +4594,7 @@
         <v>5.84</v>
       </c>
       <c r="R44" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.84</v>
       </c>
       <c r="S44" s="6">
@@ -4602,24 +4602,24 @@
         <v>2.92</v>
       </c>
       <c r="T44" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.92</v>
       </c>
       <c r="U44" s="12"/>
       <c r="V44" s="4" t="str">
-        <f>IF(NOT(M44=""),A44&amp;","&amp;M44,"")</f>
+        <f t="shared" si="18"/>
         <v>2,TC4424EPA-ND</v>
       </c>
       <c r="W44" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,TC4424EPA-ND</v>
       </c>
       <c r="X44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2x TC4424EPA</v>
       </c>
       <c r="Y44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>579-TC4424EPA|2</v>
       </c>
     </row>
@@ -4631,38 +4631,38 @@
         <v>1</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13">
         <v>1</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="N45" s="30" t="s">
-        <v>227</v>
+        <v>204</v>
+      </c>
+      <c r="N45" s="28" t="s">
+        <v>226</v>
       </c>
       <c r="O45" s="23">
         <v>0.72</v>
@@ -4675,7 +4675,7 @@
         <v>0.72</v>
       </c>
       <c r="R45" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.92</v>
       </c>
       <c r="S45" s="6">
@@ -4683,24 +4683,24 @@
         <v>0.72</v>
       </c>
       <c r="T45" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.92</v>
       </c>
       <c r="U45" s="12"/>
       <c r="V45" s="4" t="str">
-        <f t="shared" ref="V45" si="21">IF(NOT(M45=""),A45&amp;","&amp;M45,"")</f>
+        <f t="shared" ref="V45" si="26">IF(NOT(M45=""),A45&amp;","&amp;M45,"")</f>
         <v>1,ULN2803APGCN-ND</v>
       </c>
       <c r="W45" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,ULN2803APGCN-ND</v>
       </c>
       <c r="X45" t="str">
-        <f t="shared" ref="X45" si="22">A45&amp;"x "&amp;E45</f>
+        <f t="shared" ref="X45" si="27">A45&amp;"x "&amp;E45</f>
         <v>1x ULN2803APG</v>
       </c>
       <c r="Y45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>511-ULN2803A|1</v>
       </c>
     </row>
@@ -4718,7 +4718,7 @@
         <v>101</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -4726,7 +4726,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>100</v>
@@ -4735,7 +4735,7 @@
         <v>99</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O46" s="6">
         <v>0.5</v>
@@ -4748,7 +4748,7 @@
         <v>1.5</v>
       </c>
       <c r="R46" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="S46" s="6">
@@ -4756,24 +4756,24 @@
         <v>1</v>
       </c>
       <c r="T46" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="U46" s="4"/>
       <c r="V46" s="4" t="str">
-        <f>IF(NOT(M46=""),A46&amp;","&amp;M46,"")</f>
+        <f t="shared" ref="V46:V51" si="28">IF(NOT(M46=""),A46&amp;","&amp;M46,"")</f>
         <v>3,AE10011-ND</v>
       </c>
       <c r="W46" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2,AE10011-ND</v>
       </c>
       <c r="X46" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3x IC Socket</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>571-1-2199298-2|3</v>
       </c>
     </row>
@@ -4800,15 +4800,15 @@
       <c r="T47" s="6"/>
       <c r="U47" s="10"/>
       <c r="V47" s="4" t="str">
-        <f>IF(NOT(M47=""),A47&amp;","&amp;M47,"")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="W47" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -4820,10 +4820,10 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -4833,17 +4833,17 @@
         <v>1</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N48" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O48" s="6">
         <v>15.33</v>
@@ -4864,20 +4864,20 @@
         <v>15.33</v>
       </c>
       <c r="T48" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.33</v>
       </c>
       <c r="U48" s="10"/>
       <c r="V48" s="4" t="str">
-        <f>IF(NOT(M48=""),A48&amp;","&amp;M48,"")</f>
+        <f t="shared" si="28"/>
         <v>1,HM975-ND</v>
       </c>
       <c r="W48" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1,HM975-ND</v>
       </c>
       <c r="Y48" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>546-1455N1202|1</v>
       </c>
     </row>
@@ -4904,7 +4904,7 @@
       <c r="T49" s="10"/>
       <c r="U49" s="10"/>
       <c r="V49" s="4" t="str">
-        <f>IF(NOT(M49=""),A49&amp;","&amp;M49,"")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="W49" s="4" t="str">
@@ -4939,7 +4939,7 @@
       <c r="T50" s="3"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4" t="str">
-        <f>IF(NOT(M50=""),A50&amp;","&amp;M50,"")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="W50" s="4" t="str">
@@ -4953,10 +4953,10 @@
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>82</v>
@@ -4987,14 +4987,14 @@
         <v>15</v>
       </c>
       <c r="R51" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="S51" s="6"/>
       <c r="T51" s="6"/>
       <c r="U51" s="4"/>
       <c r="V51" s="4" t="str">
-        <f>IF(NOT(M51=""),A51&amp;","&amp;M51,"")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="W51" s="4"/>
@@ -5046,10 +5046,10 @@
       <c r="I53" s="8"/>
       <c r="J53" s="4"/>
       <c r="K53" s="8"/>
-      <c r="L53" s="28" t="s">
+      <c r="L53" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="M53" s="29"/>
+      <c r="M53" s="32"/>
       <c r="N53" s="27"/>
       <c r="O53" s="1" t="s">
         <v>79</v>
@@ -5057,19 +5057,19 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="11">
         <f>SUM(Q2:Q52)</f>
-        <v>103.13200000000001</v>
+        <v>102.97200000000001</v>
       </c>
       <c r="R53" s="11">
         <f>SUM(R2:R52)</f>
-        <v>105.52000000000001</v>
+        <v>105.30000000000001</v>
       </c>
       <c r="S53" s="11">
         <f>SUM(S2:S52)</f>
-        <v>76.871999999999986</v>
+        <v>76.711999999999989</v>
       </c>
       <c r="T53" s="11">
         <f>SUM(T2:T52)</f>
-        <v>81.3</v>
+        <v>81.08</v>
       </c>
       <c r="U53" s="10" t="s">
         <v>80</v>

</xml_diff>